<commit_message>
lode runner - level 1 done, 196 frames saved
</commit_message>
<xml_diff>
--- a/LodeRunner/compare.xlsx
+++ b/LodeRunner/compare.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\LodeRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D00F353-408E-4425-9DAB-77C5DFCA88BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F358B8A3-21E0-4B16-914F-17906AED1980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44115" yWindow="3675" windowWidth="11865" windowHeight="12990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="50400" yWindow="3270" windowWidth="7305" windowHeight="12990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V6" sheetId="7" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="242">
   <si>
     <t>Place</t>
   </si>
@@ -749,6 +749,18 @@
   </si>
   <si>
     <t>01 Appears (1st green)</t>
+  </si>
+  <si>
+    <t>01 1st move</t>
+  </si>
+  <si>
+    <t>gold left 4</t>
+  </si>
+  <si>
+    <t>gold left 3</t>
+  </si>
+  <si>
+    <t>gold left 2</t>
   </si>
 </sst>
 </file>
@@ -1548,11 +1560,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB48F502-AA0A-4BF9-ABA2-AA87E3F2B5E4}">
-  <dimension ref="A1:E288"/>
+  <dimension ref="A1:E291"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1587,69 +1599,77 @@
         <v>426</v>
       </c>
       <c r="D2" s="3">
-        <f t="shared" ref="D2:D34" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
+        <f t="shared" ref="D2:D37" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
-        <v>170</v>
-      </c>
-      <c r="B3" s="2"/>
+      <c r="A3" s="44" t="s">
+        <v>238</v>
+      </c>
+      <c r="B3" s="2">
+        <v>529</v>
+      </c>
       <c r="C3" s="2">
-        <v>735</v>
-      </c>
-      <c r="D3" s="3" t="str">
-        <f t="shared" ref="D3" si="1">IF(C3&lt;&gt;"",IF(B3&lt;&gt;"",C3-B3,"-"), "-")</f>
-        <v>-</v>
+        <v>736</v>
+      </c>
+      <c r="D3" s="3">
+        <f t="shared" ref="D3:D6" si="1">IF(C3&lt;&gt;"",IF(B3&lt;&gt;"",C3-B3,"-"), "-")</f>
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
-        <v>171</v>
-      </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7">
-        <v>1052</v>
-      </c>
-      <c r="D4" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A4" s="44" t="s">
+        <v>239</v>
+      </c>
+      <c r="B4" s="2">
+        <v>600</v>
+      </c>
+      <c r="C4" s="2">
+        <v>808</v>
+      </c>
+      <c r="D4" s="3">
+        <f t="shared" si="1"/>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
-        <v>172</v>
-      </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7">
-        <v>1734</v>
-      </c>
-      <c r="D5" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A5" s="44" t="s">
+        <v>240</v>
+      </c>
+      <c r="B5" s="2">
+        <v>628</v>
+      </c>
+      <c r="C5" s="2">
+        <v>840</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" si="1"/>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="33" t="s">
-        <v>173</v>
-      </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7">
-        <v>2189</v>
-      </c>
-      <c r="D6" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A6" s="44" t="s">
+        <v>241</v>
+      </c>
+      <c r="B6" s="2">
+        <v>663</v>
+      </c>
+      <c r="C6" s="2">
+        <v>872</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" si="1"/>
+        <v>209</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7">
-        <v>2835</v>
+        <v>1052</v>
       </c>
       <c r="D7" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1658,11 +1678,11 @@
     </row>
     <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="7">
-        <v>3256</v>
+        <v>1734</v>
       </c>
       <c r="D8" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1671,11 +1691,11 @@
     </row>
     <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="7">
-        <v>3901</v>
+        <v>2189</v>
       </c>
       <c r="D9" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1684,11 +1704,11 @@
     </row>
     <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="7">
-        <v>4382</v>
+        <v>2835</v>
       </c>
       <c r="D10" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1697,11 +1717,11 @@
     </row>
     <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="33" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7">
-        <v>5042</v>
+        <v>3256</v>
       </c>
       <c r="D11" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1710,11 +1730,11 @@
     </row>
     <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="33" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="7">
-        <v>5332</v>
+        <v>3901</v>
       </c>
       <c r="D12" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1723,11 +1743,11 @@
     </row>
     <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="7">
-        <v>5978</v>
+        <v>4382</v>
       </c>
       <c r="D13" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1736,11 +1756,11 @@
     </row>
     <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="7">
-        <v>6999</v>
+        <v>5042</v>
       </c>
       <c r="D14" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1749,11 +1769,11 @@
     </row>
     <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="7">
-        <v>7646</v>
+        <v>5332</v>
       </c>
       <c r="D15" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1762,11 +1782,11 @@
     </row>
     <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="33" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B16" s="7"/>
       <c r="C16" s="7">
-        <v>8112</v>
+        <v>5978</v>
       </c>
       <c r="D16" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1775,11 +1795,11 @@
     </row>
     <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="33" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B17" s="7"/>
       <c r="C17" s="7">
-        <v>8758</v>
+        <v>6999</v>
       </c>
       <c r="D17" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1788,11 +1808,11 @@
     </row>
     <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="33" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B18" s="7"/>
       <c r="C18" s="7">
-        <v>9166</v>
+        <v>7646</v>
       </c>
       <c r="D18" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1801,11 +1821,11 @@
     </row>
     <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="33" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B19" s="7"/>
       <c r="C19" s="7">
-        <v>9811</v>
+        <v>8112</v>
       </c>
       <c r="D19" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1814,11 +1834,11 @@
     </row>
     <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="33" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="7">
-        <v>10903</v>
+        <v>8758</v>
       </c>
       <c r="D20" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1827,11 +1847,11 @@
     </row>
     <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="33" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B21" s="7"/>
       <c r="C21" s="7">
-        <v>11541</v>
+        <v>9166</v>
       </c>
       <c r="D21" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1840,11 +1860,11 @@
     </row>
     <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="33" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B22" s="7"/>
       <c r="C22" s="7">
-        <v>12111</v>
+        <v>9811</v>
       </c>
       <c r="D22" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1853,11 +1873,11 @@
     </row>
     <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="33" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B23" s="7"/>
       <c r="C23" s="7">
-        <v>12770</v>
+        <v>10903</v>
       </c>
       <c r="D23" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1866,11 +1886,11 @@
     </row>
     <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="33" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B24" s="7"/>
       <c r="C24" s="7">
-        <v>13076</v>
+        <v>11541</v>
       </c>
       <c r="D24" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1879,11 +1899,11 @@
     </row>
     <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="33" t="s">
-        <v>192</v>
-      </c>
-      <c r="B25" s="33"/>
-      <c r="C25" s="33">
-        <v>13735</v>
+        <v>189</v>
+      </c>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7">
+        <v>12111</v>
       </c>
       <c r="D25" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1892,11 +1912,11 @@
     </row>
     <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="33" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B26" s="7"/>
       <c r="C26" s="7">
-        <v>14417</v>
+        <v>12770</v>
       </c>
       <c r="D26" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1905,11 +1925,11 @@
     </row>
     <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="33" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B27" s="7"/>
       <c r="C27" s="7">
-        <v>15063</v>
+        <v>13076</v>
       </c>
       <c r="D27" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1917,12 +1937,12 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7">
-        <v>15660</v>
+      <c r="A28" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="B28" s="33"/>
+      <c r="C28" s="33">
+        <v>13735</v>
       </c>
       <c r="D28" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1930,12 +1950,12 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
-        <v>196</v>
+      <c r="A29" s="33" t="s">
+        <v>193</v>
       </c>
       <c r="B29" s="7"/>
       <c r="C29" s="7">
-        <v>16305</v>
+        <v>14417</v>
       </c>
       <c r="D29" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1943,12 +1963,12 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
-        <v>195</v>
+      <c r="A30" s="33" t="s">
+        <v>194</v>
       </c>
       <c r="B30" s="7"/>
       <c r="C30" s="7">
-        <v>16830</v>
+        <v>15063</v>
       </c>
       <c r="D30" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1956,12 +1976,12 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
-        <v>197</v>
+      <c r="A31" s="8" t="s">
+        <v>195</v>
       </c>
       <c r="B31" s="7"/>
       <c r="C31" s="7">
-        <v>17476</v>
+        <v>15660</v>
       </c>
       <c r="D31" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1970,11 +1990,11 @@
     </row>
     <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B32" s="7"/>
       <c r="C32" s="7">
-        <v>18217</v>
+        <v>16305</v>
       </c>
       <c r="D32" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1983,91 +2003,91 @@
     </row>
     <row r="33" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B33" s="7"/>
       <c r="C33" s="7">
-        <v>18855</v>
+        <v>16830</v>
       </c>
       <c r="D33" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E33" s="7"/>
     </row>
     <row r="34" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B34" s="7"/>
       <c r="C34" s="7">
-        <v>19222</v>
+        <v>17476</v>
       </c>
       <c r="D34" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E34" s="7"/>
     </row>
     <row r="35" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B35" s="7"/>
       <c r="C35" s="7">
-        <v>19867</v>
+        <v>18217</v>
       </c>
       <c r="D35" s="3" t="str">
-        <f t="shared" ref="D35:D66" si="2">IF(C35&lt;&gt;"",IF(B35&lt;&gt;"",C35-B35,"-"), "-")</f>
+        <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="33" t="s">
-        <v>232</v>
+      <c r="A36" s="7" t="s">
+        <v>199</v>
       </c>
       <c r="B36" s="7"/>
       <c r="C36" s="7">
-        <v>20034</v>
+        <v>18855</v>
       </c>
       <c r="D36" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="E36" s="7"/>
     </row>
     <row r="37" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B37" s="7"/>
       <c r="C37" s="7">
-        <v>20738</v>
+        <v>19222</v>
       </c>
       <c r="D37" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="E37" s="7"/>
     </row>
     <row r="38" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B38" s="7"/>
       <c r="C38" s="7">
-        <v>21383</v>
+        <v>19867</v>
       </c>
       <c r="D38" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="D38:D69" si="2">IF(C38&lt;&gt;"",IF(B38&lt;&gt;"",C38-B38,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8">
-        <v>22330</v>
+      <c r="A39" s="33" t="s">
+        <v>232</v>
+      </c>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7">
+        <v>20034</v>
       </c>
       <c r="D39" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2076,11 +2096,11 @@
     </row>
     <row r="40" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="B40" s="33"/>
-      <c r="C40" s="33">
-        <v>22994</v>
+        <v>202</v>
+      </c>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7">
+        <v>20738</v>
       </c>
       <c r="D40" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2089,11 +2109,11 @@
     </row>
     <row r="41" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B41" s="7"/>
       <c r="C41" s="7">
-        <v>23293</v>
+        <v>21383</v>
       </c>
       <c r="D41" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2102,11 +2122,11 @@
     </row>
     <row r="42" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7">
-        <v>23953</v>
+        <v>204</v>
+      </c>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8">
+        <v>22330</v>
       </c>
       <c r="D42" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2115,11 +2135,11 @@
     </row>
     <row r="43" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="B43" s="7"/>
-      <c r="C43" s="7">
-        <v>24530</v>
+        <v>205</v>
+      </c>
+      <c r="B43" s="33"/>
+      <c r="C43" s="33">
+        <v>22994</v>
       </c>
       <c r="D43" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2128,11 +2148,11 @@
     </row>
     <row r="44" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B44" s="7"/>
       <c r="C44" s="7">
-        <v>25190</v>
+        <v>23293</v>
       </c>
       <c r="D44" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2141,11 +2161,11 @@
     </row>
     <row r="45" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B45" s="7"/>
       <c r="C45" s="7">
-        <v>26022</v>
+        <v>23953</v>
       </c>
       <c r="D45" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2154,11 +2174,11 @@
     </row>
     <row r="46" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B46" s="7"/>
       <c r="C46" s="7">
-        <v>26681</v>
+        <v>24530</v>
       </c>
       <c r="D46" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2167,11 +2187,11 @@
     </row>
     <row r="47" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B47" s="7"/>
       <c r="C47" s="7">
-        <v>27241</v>
+        <v>25190</v>
       </c>
       <c r="D47" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2180,11 +2200,11 @@
     </row>
     <row r="48" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B48" s="7"/>
       <c r="C48" s="7">
-        <v>27889</v>
+        <v>26022</v>
       </c>
       <c r="D48" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2193,11 +2213,11 @@
     </row>
     <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B49" s="7"/>
       <c r="C49" s="7">
-        <v>28945</v>
+        <v>26681</v>
       </c>
       <c r="D49" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2206,11 +2226,11 @@
     </row>
     <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B50" s="7"/>
       <c r="C50" s="7">
-        <v>29444</v>
+        <v>27241</v>
       </c>
       <c r="D50" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2219,11 +2239,11 @@
     </row>
     <row r="51" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B51" s="7"/>
       <c r="C51" s="7">
-        <v>29868</v>
+        <v>27889</v>
       </c>
       <c r="D51" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2232,11 +2252,11 @@
     </row>
     <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B52" s="7"/>
       <c r="C52" s="7">
-        <v>30507</v>
+        <v>28945</v>
       </c>
       <c r="D52" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2245,11 +2265,11 @@
     </row>
     <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B53" s="7"/>
       <c r="C53" s="7">
-        <v>31061</v>
+        <v>29444</v>
       </c>
       <c r="D53" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2258,11 +2278,11 @@
     </row>
     <row r="54" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B54" s="7"/>
       <c r="C54" s="7">
-        <v>31706</v>
+        <v>29868</v>
       </c>
       <c r="D54" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2271,11 +2291,11 @@
     </row>
     <row r="55" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B55" s="7"/>
       <c r="C55" s="7">
-        <v>32622</v>
+        <v>30507</v>
       </c>
       <c r="D55" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2284,11 +2304,11 @@
     </row>
     <row r="56" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B56" s="7"/>
       <c r="C56" s="7">
-        <v>33269</v>
+        <v>31061</v>
       </c>
       <c r="D56" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2297,11 +2317,11 @@
     </row>
     <row r="57" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B57" s="7"/>
       <c r="C57" s="7">
-        <v>34177</v>
+        <v>31706</v>
       </c>
       <c r="D57" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2310,11 +2330,11 @@
     </row>
     <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B58" s="7"/>
       <c r="C58" s="7">
-        <v>34821</v>
+        <v>32622</v>
       </c>
       <c r="D58" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2323,11 +2343,11 @@
     </row>
     <row r="59" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B59" s="7"/>
       <c r="C59" s="7">
-        <v>35636</v>
+        <v>33269</v>
       </c>
       <c r="D59" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2336,11 +2356,11 @@
     </row>
     <row r="60" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B60" s="7"/>
       <c r="C60" s="7">
-        <v>36237</v>
+        <v>34177</v>
       </c>
       <c r="D60" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2349,11 +2369,11 @@
     </row>
     <row r="61" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>27</v>
+        <v>223</v>
       </c>
       <c r="B61" s="7"/>
       <c r="C61" s="7">
-        <v>37327</v>
+        <v>34821</v>
       </c>
       <c r="D61" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2362,11 +2382,11 @@
     </row>
     <row r="62" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B62" s="7"/>
       <c r="C62" s="7">
-        <v>37819</v>
+        <v>35636</v>
       </c>
       <c r="D62" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2374,12 +2394,12 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A63" s="34" t="s">
-        <v>234</v>
+      <c r="A63" s="7" t="s">
+        <v>225</v>
       </c>
       <c r="B63" s="7"/>
       <c r="C63" s="7">
-        <v>38071</v>
+        <v>36237</v>
       </c>
       <c r="D63" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2387,12 +2407,12 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A64" s="34" t="s">
-        <v>233</v>
+      <c r="A64" s="7" t="s">
+        <v>27</v>
       </c>
       <c r="B64" s="7"/>
       <c r="C64" s="7">
-        <v>38132</v>
+        <v>37327</v>
       </c>
       <c r="D64" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2400,12 +2420,12 @@
       </c>
     </row>
     <row r="65" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A65" s="34" t="s">
-        <v>150</v>
+      <c r="A65" s="7" t="s">
+        <v>226</v>
       </c>
       <c r="B65" s="7"/>
       <c r="C65" s="7">
-        <v>38145</v>
+        <v>37819</v>
       </c>
       <c r="D65" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2413,12 +2433,12 @@
       </c>
     </row>
     <row r="66" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A66" s="7" t="s">
-        <v>227</v>
+      <c r="A66" s="34" t="s">
+        <v>234</v>
       </c>
       <c r="B66" s="7"/>
       <c r="C66" s="7">
-        <v>38527</v>
+        <v>38071</v>
       </c>
       <c r="D66" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2426,64 +2446,64 @@
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A67" s="7" t="s">
-        <v>228</v>
+      <c r="A67" s="34" t="s">
+        <v>233</v>
       </c>
       <c r="B67" s="7"/>
       <c r="C67" s="7">
-        <v>39151</v>
+        <v>38132</v>
       </c>
       <c r="D67" s="3" t="str">
-        <f t="shared" ref="D67:D98" si="3">IF(C67&lt;&gt;"",IF(B67&lt;&gt;"",C67-B67,"-"), "-")</f>
+        <f t="shared" si="2"/>
         <v>-</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A68" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="B68" s="9"/>
-      <c r="C68" s="9">
-        <v>39334</v>
+      <c r="A68" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="B68" s="7"/>
+      <c r="C68" s="7">
+        <v>38145</v>
       </c>
       <c r="D68" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B69" s="7"/>
       <c r="C69" s="7">
-        <v>39973</v>
+        <v>38527</v>
       </c>
       <c r="D69" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="B70" s="9"/>
-      <c r="C70" s="9">
-        <v>40494</v>
+        <v>228</v>
+      </c>
+      <c r="B70" s="7"/>
+      <c r="C70" s="7">
+        <v>39151</v>
       </c>
       <c r="D70" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="D70:D101" si="3">IF(C70&lt;&gt;"",IF(B70&lt;&gt;"",C70-B70,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="B71" s="7"/>
-      <c r="C71" s="7">
-        <v>41139</v>
+        <v>229</v>
+      </c>
+      <c r="B71" s="9"/>
+      <c r="C71" s="9">
+        <v>39334</v>
       </c>
       <c r="D71" s="3" t="str">
         <f t="shared" si="3"/>
@@ -2492,11 +2512,11 @@
     </row>
     <row r="72" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
-        <v>124</v>
+        <v>230</v>
       </c>
       <c r="B72" s="7"/>
       <c r="C72" s="7">
-        <v>41742</v>
+        <v>39973</v>
       </c>
       <c r="D72" s="3" t="str">
         <f t="shared" si="3"/>
@@ -2504,12 +2524,12 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A73" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B73" s="7"/>
-      <c r="C73" s="7">
-        <v>42387</v>
+      <c r="A73" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B73" s="9"/>
+      <c r="C73" s="9">
+        <v>40494</v>
       </c>
       <c r="D73" s="3" t="str">
         <f t="shared" si="3"/>
@@ -2517,64 +2537,64 @@
       </c>
     </row>
     <row r="74" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A74" s="5" t="s">
-        <v>31</v>
+      <c r="A74" s="7" t="s">
+        <v>123</v>
       </c>
       <c r="B74" s="7"/>
       <c r="C74" s="7">
-        <v>43033</v>
+        <v>41139</v>
       </c>
       <c r="D74" s="3" t="str">
-        <f t="shared" ref="D74:D142" si="4">IF(C74&lt;&gt;"",IF(B74&lt;&gt;"",C74-B74,"-"), "-")</f>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A75" s="5" t="s">
-        <v>11</v>
+      <c r="A75" s="7" t="s">
+        <v>124</v>
       </c>
       <c r="B75" s="7"/>
       <c r="C75" s="7">
-        <v>43693</v>
+        <v>41742</v>
       </c>
       <c r="D75" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="B76" s="7"/>
       <c r="C76" s="7">
-        <v>44329</v>
+        <v>42387</v>
       </c>
       <c r="D76" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="B77" s="7"/>
       <c r="C77" s="7">
-        <v>44988</v>
+        <v>43033</v>
       </c>
       <c r="D77" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="D77:D145" si="4">IF(C77&lt;&gt;"",IF(B77&lt;&gt;"",C77-B77,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="B78" s="7"/>
       <c r="C78" s="7">
-        <v>45587</v>
+        <v>43693</v>
       </c>
       <c r="D78" s="3" t="str">
         <f t="shared" si="4"/>
@@ -2583,11 +2603,11 @@
     </row>
     <row r="79" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="B79" s="7"/>
       <c r="C79" s="7">
-        <v>46248</v>
+        <v>44329</v>
       </c>
       <c r="D79" s="3" t="str">
         <f t="shared" si="4"/>
@@ -2595,12 +2615,12 @@
       </c>
     </row>
     <row r="80" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A80" s="7" t="s">
-        <v>47</v>
+      <c r="A80" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="B80" s="7"/>
       <c r="C80" s="7">
-        <v>47029</v>
+        <v>44988</v>
       </c>
       <c r="D80" s="3" t="str">
         <f t="shared" si="4"/>
@@ -2608,12 +2628,12 @@
       </c>
     </row>
     <row r="81" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A81" s="7" t="s">
-        <v>48</v>
+      <c r="A81" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="B81" s="7"/>
       <c r="C81" s="7">
-        <v>47527</v>
+        <v>45587</v>
       </c>
       <c r="D81" s="3" t="str">
         <f t="shared" si="4"/>
@@ -2621,12 +2641,12 @@
       </c>
     </row>
     <row r="82" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A82" s="34" t="s">
-        <v>235</v>
+      <c r="A82" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="B82" s="7"/>
       <c r="C82" s="7">
-        <v>48010</v>
+        <v>46248</v>
       </c>
       <c r="D82" s="3" t="str">
         <f t="shared" si="4"/>
@@ -2635,11 +2655,11 @@
     </row>
     <row r="83" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="B83" s="7"/>
       <c r="C83" s="7">
-        <v>48393</v>
+        <v>47029</v>
       </c>
       <c r="D83" s="3" t="str">
         <f t="shared" si="4"/>
@@ -2647,12 +2667,12 @@
       </c>
     </row>
     <row r="84" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A84" s="5" t="s">
-        <v>14</v>
+      <c r="A84" s="7" t="s">
+        <v>48</v>
       </c>
       <c r="B84" s="7"/>
       <c r="C84" s="7">
-        <v>49053</v>
+        <v>47527</v>
       </c>
       <c r="D84" s="3" t="str">
         <f t="shared" si="4"/>
@@ -2660,12 +2680,12 @@
       </c>
     </row>
     <row r="85" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A85" s="5" t="s">
-        <v>34</v>
+      <c r="A85" s="34" t="s">
+        <v>235</v>
       </c>
       <c r="B85" s="7"/>
       <c r="C85" s="7">
-        <v>49311</v>
+        <v>48010</v>
       </c>
       <c r="D85" s="3" t="str">
         <f t="shared" si="4"/>
@@ -2673,12 +2693,12 @@
       </c>
     </row>
     <row r="86" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A86" s="5" t="s">
-        <v>15</v>
+      <c r="A86" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="B86" s="7"/>
       <c r="C86" s="7">
-        <v>49911</v>
+        <v>48393</v>
       </c>
       <c r="D86" s="3" t="str">
         <f t="shared" si="4"/>
@@ -2687,11 +2707,11 @@
     </row>
     <row r="87" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="B87" s="7"/>
       <c r="C87" s="7">
-        <v>50889</v>
+        <v>49053</v>
       </c>
       <c r="D87" s="3" t="str">
         <f t="shared" si="4"/>
@@ -2700,11 +2720,11 @@
     </row>
     <row r="88" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="B88" s="7"/>
       <c r="C88" s="7">
-        <v>51535</v>
+        <v>49311</v>
       </c>
       <c r="D88" s="3" t="str">
         <f t="shared" si="4"/>
@@ -2713,11 +2733,11 @@
     </row>
     <row r="89" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="B89" s="7"/>
       <c r="C89" s="7">
-        <v>52312</v>
+        <v>49911</v>
       </c>
       <c r="D89" s="3" t="str">
         <f t="shared" si="4"/>
@@ -2726,11 +2746,11 @@
     </row>
     <row r="90" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="B90" s="7"/>
       <c r="C90" s="7">
-        <v>52934</v>
+        <v>50889</v>
       </c>
       <c r="D90" s="3" t="str">
         <f t="shared" si="4"/>
@@ -2739,11 +2759,11 @@
     </row>
     <row r="91" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="B91" s="7"/>
       <c r="C91" s="7">
-        <v>53936</v>
+        <v>51535</v>
       </c>
       <c r="D91" s="3" t="str">
         <f t="shared" si="4"/>
@@ -2752,11 +2772,11 @@
     </row>
     <row r="92" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="B92" s="7"/>
       <c r="C92" s="7">
-        <v>54526</v>
+        <v>52312</v>
       </c>
       <c r="D92" s="3" t="str">
         <f t="shared" si="4"/>
@@ -2765,11 +2785,11 @@
     </row>
     <row r="93" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="B93" s="7"/>
       <c r="C93" s="7">
-        <v>54878</v>
+        <v>52934</v>
       </c>
       <c r="D93" s="3" t="str">
         <f t="shared" si="4"/>
@@ -2778,11 +2798,11 @@
     </row>
     <row r="94" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="B94" s="7"/>
       <c r="C94" s="7">
-        <v>55524</v>
+        <v>53936</v>
       </c>
       <c r="D94" s="3" t="str">
         <f t="shared" si="4"/>
@@ -2791,11 +2811,11 @@
     </row>
     <row r="95" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="B95" s="7"/>
       <c r="C95" s="7">
-        <v>56204</v>
+        <v>54526</v>
       </c>
       <c r="D95" s="3" t="str">
         <f t="shared" si="4"/>
@@ -2804,11 +2824,11 @@
     </row>
     <row r="96" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="B96" s="7"/>
       <c r="C96" s="7">
-        <v>56804</v>
+        <v>54878</v>
       </c>
       <c r="D96" s="3" t="str">
         <f t="shared" si="4"/>
@@ -2817,11 +2837,11 @@
     </row>
     <row r="97" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="B97" s="7"/>
       <c r="C97" s="7">
-        <v>57359</v>
+        <v>55524</v>
       </c>
       <c r="D97" s="3" t="str">
         <f t="shared" si="4"/>
@@ -2830,11 +2850,11 @@
     </row>
     <row r="98" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="B98" s="7"/>
       <c r="C98" s="7">
-        <v>57995</v>
+        <v>56204</v>
       </c>
       <c r="D98" s="3" t="str">
         <f t="shared" si="4"/>
@@ -2843,11 +2863,11 @@
     </row>
     <row r="99" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="B99" s="7"/>
       <c r="C99" s="7">
-        <v>58575</v>
+        <v>56804</v>
       </c>
       <c r="D99" s="3" t="str">
         <f t="shared" si="4"/>
@@ -2856,11 +2876,11 @@
     </row>
     <row r="100" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="B100" s="7"/>
       <c r="C100" s="7">
-        <v>59227</v>
+        <v>57359</v>
       </c>
       <c r="D100" s="3" t="str">
         <f t="shared" si="4"/>
@@ -2869,11 +2889,11 @@
     </row>
     <row r="101" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B101" s="10"/>
-      <c r="C101" s="10">
-        <v>60018</v>
+        <v>21</v>
+      </c>
+      <c r="B101" s="7"/>
+      <c r="C101" s="7">
+        <v>57995</v>
       </c>
       <c r="D101" s="3" t="str">
         <f t="shared" si="4"/>
@@ -2882,11 +2902,11 @@
     </row>
     <row r="102" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="B102" s="7"/>
       <c r="C102" s="7">
-        <v>60663</v>
+        <v>58575</v>
       </c>
       <c r="D102" s="3" t="str">
         <f t="shared" si="4"/>
@@ -2894,12 +2914,12 @@
       </c>
     </row>
     <row r="103" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A103" s="35" t="s">
-        <v>127</v>
+      <c r="A103" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="B103" s="7"/>
       <c r="C103" s="7">
-        <v>60822</v>
+        <v>59227</v>
       </c>
       <c r="D103" s="3" t="str">
         <f t="shared" si="4"/>
@@ -2908,11 +2928,11 @@
     </row>
     <row r="104" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B104" s="7"/>
-      <c r="C104" s="7">
-        <v>61231</v>
+        <v>42</v>
+      </c>
+      <c r="B104" s="10"/>
+      <c r="C104" s="10">
+        <v>60018</v>
       </c>
       <c r="D104" s="3" t="str">
         <f t="shared" si="4"/>
@@ -2921,11 +2941,11 @@
     </row>
     <row r="105" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B105" s="7"/>
       <c r="C105" s="7">
-        <v>61891</v>
+        <v>60663</v>
       </c>
       <c r="D105" s="3" t="str">
         <f t="shared" si="4"/>
@@ -2933,12 +2953,12 @@
       </c>
     </row>
     <row r="106" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A106" s="5" t="s">
-        <v>44</v>
+      <c r="A106" s="35" t="s">
+        <v>127</v>
       </c>
       <c r="B106" s="7"/>
       <c r="C106" s="7">
-        <v>62598</v>
+        <v>60822</v>
       </c>
       <c r="D106" s="3" t="str">
         <f t="shared" si="4"/>
@@ -2947,11 +2967,11 @@
     </row>
     <row r="107" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="B107" s="7"/>
       <c r="C107" s="7">
-        <v>63243</v>
+        <v>61231</v>
       </c>
       <c r="D107" s="3" t="str">
         <f t="shared" si="4"/>
@@ -2959,64 +2979,76 @@
       </c>
     </row>
     <row r="108" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A108" s="5"/>
+      <c r="A108" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="B108" s="7"/>
       <c r="C108" s="7">
-        <v>63497</v>
-      </c>
-      <c r="D108" s="3"/>
+        <v>61891</v>
+      </c>
+      <c r="D108" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="109" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A109" s="5"/>
+      <c r="A109" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="B109" s="7"/>
       <c r="C109" s="7">
-        <v>63552</v>
-      </c>
-      <c r="D109" s="3"/>
+        <v>62598</v>
+      </c>
+      <c r="D109" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="110" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A110" s="5"/>
+      <c r="A110" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="B110" s="7"/>
       <c r="C110" s="7">
-        <v>63603</v>
-      </c>
-      <c r="D110" s="3"/>
+        <v>63243</v>
+      </c>
+      <c r="D110" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="111" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A111" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="A111" s="5"/>
       <c r="B111" s="7"/>
       <c r="C111" s="7">
+        <v>63497</v>
+      </c>
+      <c r="D111" s="3"/>
+    </row>
+    <row r="112" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A112" s="5"/>
+      <c r="B112" s="7"/>
+      <c r="C112" s="7">
+        <v>63552</v>
+      </c>
+      <c r="D112" s="3"/>
+    </row>
+    <row r="113" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A113" s="5"/>
+      <c r="B113" s="7"/>
+      <c r="C113" s="7">
+        <v>63603</v>
+      </c>
+      <c r="D113" s="3"/>
+    </row>
+    <row r="114" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A114" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B114" s="7"/>
+      <c r="C114" s="7">
         <v>63782</v>
       </c>
-      <c r="D111" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A112" s="7"/>
-      <c r="B112" s="7"/>
-      <c r="C112" s="7"/>
-      <c r="D112" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A113" s="7"/>
-      <c r="B113" s="7"/>
-      <c r="C113" s="7"/>
-      <c r="D113" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A114" s="7"/>
-      <c r="B114" s="7"/>
-      <c r="C114" s="7"/>
       <c r="D114" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
@@ -3279,7 +3311,7 @@
       <c r="B143" s="7"/>
       <c r="C143" s="7"/>
       <c r="D143" s="3" t="str">
-        <f t="shared" ref="D143:D147" si="5">IF(C143&lt;&gt;"",IF(B143&lt;&gt;"",C143-B143,"-"), "-")</f>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
     </row>
@@ -3288,7 +3320,7 @@
       <c r="B144" s="7"/>
       <c r="C144" s="7"/>
       <c r="D144" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
     </row>
@@ -3297,7 +3329,7 @@
       <c r="B145" s="7"/>
       <c r="C145" s="7"/>
       <c r="D145" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
     </row>
@@ -3306,7 +3338,7 @@
       <c r="B146" s="7"/>
       <c r="C146" s="7"/>
       <c r="D146" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="D146:D150" si="5">IF(C146&lt;&gt;"",IF(B146&lt;&gt;"",C146-B146,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
@@ -3324,7 +3356,7 @@
       <c r="B148" s="7"/>
       <c r="C148" s="7"/>
       <c r="D148" s="3" t="str">
-        <f t="shared" ref="D148:D149" si="6">IF(C148&lt;&gt;"",IF(B148&lt;&gt;"",B148-C148,"-"), "-")</f>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
     </row>
@@ -3333,7 +3365,7 @@
       <c r="B149" s="7"/>
       <c r="C149" s="7"/>
       <c r="D149" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
     </row>
@@ -3341,21 +3373,36 @@
       <c r="A150" s="7"/>
       <c r="B150" s="7"/>
       <c r="C150" s="7"/>
+      <c r="D150" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="151" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A151" s="7"/>
       <c r="B151" s="7"/>
       <c r="C151" s="7"/>
+      <c r="D151" s="3" t="str">
+        <f t="shared" ref="D151:D152" si="6">IF(C151&lt;&gt;"",IF(B151&lt;&gt;"",B151-C151,"-"), "-")</f>
+        <v>-</v>
+      </c>
     </row>
     <row r="152" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A152" s="7"/>
       <c r="B152" s="7"/>
       <c r="C152" s="7"/>
+      <c r="D152" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="153" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A153" s="7"/>
       <c r="B153" s="7"/>
       <c r="C153" s="7"/>
     </row>
     <row r="154" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A154" s="7"/>
       <c r="B154" s="7"/>
       <c r="C154" s="7"/>
     </row>
@@ -3894,6 +3941,18 @@
     <row r="288" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B288" s="7"/>
       <c r="C288" s="7"/>
+    </row>
+    <row r="289" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B289" s="7"/>
+      <c r="C289" s="7"/>
+    </row>
+    <row r="290" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B290" s="7"/>
+      <c r="C290" s="7"/>
+    </row>
+    <row r="291" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B291" s="7"/>
+      <c r="C291" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
better level 1 scroll skip, no use of pause, 296 ahead at the end of level 1
</commit_message>
<xml_diff>
--- a/LodeRunner/compare.xlsx
+++ b/LodeRunner/compare.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\LodeRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F358B8A3-21E0-4B16-914F-17906AED1980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C7F00D3-00C6-48BA-BE05-ABEB53498FE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="50400" yWindow="3270" windowWidth="7305" windowHeight="12990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="50280" yWindow="3255" windowWidth="7305" windowHeight="12990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V6" sheetId="7" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="244">
   <si>
     <t>Place</t>
   </si>
@@ -761,6 +761,12 @@
   </si>
   <si>
     <t>gold left 2</t>
+  </si>
+  <si>
+    <t>01 End (lag frame)</t>
+  </si>
+  <si>
+    <t>02 1st move</t>
   </si>
 </sst>
 </file>
@@ -770,12 +776,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]&quot;-&quot;[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1123,120 +1136,121 @@
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1560,11 +1574,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB48F502-AA0A-4BF9-ABA2-AA87E3F2B5E4}">
-  <dimension ref="A1:E291"/>
+  <dimension ref="A1:E292"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1589,7 +1603,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="36" t="s">
         <v>237</v>
       </c>
       <c r="B2" s="2">
@@ -1599,12 +1613,12 @@
         <v>426</v>
       </c>
       <c r="D2" s="3">
-        <f t="shared" ref="D2:D37" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
+        <f t="shared" ref="D2:D38" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="36" t="s">
         <v>238</v>
       </c>
       <c r="B3" s="2">
@@ -1614,12 +1628,12 @@
         <v>736</v>
       </c>
       <c r="D3" s="3">
-        <f t="shared" ref="D3:D6" si="1">IF(C3&lt;&gt;"",IF(B3&lt;&gt;"",C3-B3,"-"), "-")</f>
+        <f t="shared" ref="D3:D7" si="1">IF(C3&lt;&gt;"",IF(B3&lt;&gt;"",C3-B3,"-"), "-")</f>
         <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="36" t="s">
         <v>239</v>
       </c>
       <c r="B4" s="2">
@@ -1634,7 +1648,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="36" t="s">
         <v>240</v>
       </c>
       <c r="B5" s="2">
@@ -1649,7 +1663,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="36" t="s">
         <v>241</v>
       </c>
       <c r="B6" s="2">
@@ -1664,38 +1678,40 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="33" t="s">
-        <v>171</v>
-      </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7">
-        <v>1052</v>
-      </c>
-      <c r="D7" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A7" s="36"/>
+      <c r="B7" s="2">
+        <v>812</v>
+      </c>
+      <c r="C7" s="2">
+        <v>999</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="1"/>
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
-        <v>172</v>
-      </c>
-      <c r="B8" s="7"/>
+      <c r="A8" s="36" t="s">
+        <v>242</v>
+      </c>
+      <c r="B8" s="7">
+        <v>753</v>
+      </c>
       <c r="C8" s="7">
-        <v>1734</v>
-      </c>
-      <c r="D8" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>1049</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" si="0"/>
+        <v>296</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="33" t="s">
-        <v>173</v>
+      <c r="A9" s="45" t="s">
+        <v>243</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="7">
-        <v>2189</v>
+        <v>1704</v>
       </c>
       <c r="D9" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1704,12 +1720,10 @@
     </row>
     <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B10" s="7"/>
-      <c r="C10" s="7">
-        <v>2835</v>
-      </c>
+      <c r="C10" s="7"/>
       <c r="D10" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1717,12 +1731,10 @@
     </row>
     <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="33" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B11" s="7"/>
-      <c r="C11" s="7">
-        <v>3256</v>
-      </c>
+      <c r="C11" s="7"/>
       <c r="D11" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1730,12 +1742,10 @@
     </row>
     <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="33" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B12" s="7"/>
-      <c r="C12" s="7">
-        <v>3901</v>
-      </c>
+      <c r="C12" s="7"/>
       <c r="D12" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1743,12 +1753,10 @@
     </row>
     <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B13" s="7"/>
-      <c r="C13" s="7">
-        <v>4382</v>
-      </c>
+      <c r="C13" s="7"/>
       <c r="D13" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1756,12 +1764,10 @@
     </row>
     <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B14" s="7"/>
-      <c r="C14" s="7">
-        <v>5042</v>
-      </c>
+      <c r="C14" s="7"/>
       <c r="D14" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1769,12 +1775,10 @@
     </row>
     <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B15" s="7"/>
-      <c r="C15" s="7">
-        <v>5332</v>
-      </c>
+      <c r="C15" s="7"/>
       <c r="D15" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1782,12 +1786,10 @@
     </row>
     <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="33" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B16" s="7"/>
-      <c r="C16" s="7">
-        <v>5978</v>
-      </c>
+      <c r="C16" s="7"/>
       <c r="D16" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1795,12 +1797,10 @@
     </row>
     <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="33" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B17" s="7"/>
-      <c r="C17" s="7">
-        <v>6999</v>
-      </c>
+      <c r="C17" s="7"/>
       <c r="D17" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1808,12 +1808,10 @@
     </row>
     <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="33" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B18" s="7"/>
-      <c r="C18" s="7">
-        <v>7646</v>
-      </c>
+      <c r="C18" s="7"/>
       <c r="D18" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1821,12 +1819,10 @@
     </row>
     <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B19" s="7"/>
-      <c r="C19" s="7">
-        <v>8112</v>
-      </c>
+      <c r="C19" s="7"/>
       <c r="D19" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1834,12 +1830,10 @@
     </row>
     <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="33" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B20" s="7"/>
-      <c r="C20" s="7">
-        <v>8758</v>
-      </c>
+      <c r="C20" s="7"/>
       <c r="D20" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1847,12 +1841,10 @@
     </row>
     <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="33" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B21" s="7"/>
-      <c r="C21" s="7">
-        <v>9166</v>
-      </c>
+      <c r="C21" s="7"/>
       <c r="D21" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1860,12 +1852,10 @@
     </row>
     <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="33" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B22" s="7"/>
-      <c r="C22" s="7">
-        <v>9811</v>
-      </c>
+      <c r="C22" s="7"/>
       <c r="D22" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1873,12 +1863,10 @@
     </row>
     <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="33" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B23" s="7"/>
-      <c r="C23" s="7">
-        <v>10903</v>
-      </c>
+      <c r="C23" s="7"/>
       <c r="D23" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1886,12 +1874,10 @@
     </row>
     <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B24" s="7"/>
-      <c r="C24" s="7">
-        <v>11541</v>
-      </c>
+      <c r="C24" s="7"/>
       <c r="D24" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1899,12 +1885,10 @@
     </row>
     <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="33" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B25" s="7"/>
-      <c r="C25" s="7">
-        <v>12111</v>
-      </c>
+      <c r="C25" s="7"/>
       <c r="D25" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1912,12 +1896,10 @@
     </row>
     <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="33" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B26" s="7"/>
-      <c r="C26" s="7">
-        <v>12770</v>
-      </c>
+      <c r="C26" s="7"/>
       <c r="D26" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1925,12 +1907,10 @@
     </row>
     <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="33" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B27" s="7"/>
-      <c r="C27" s="7">
-        <v>13076</v>
-      </c>
+      <c r="C27" s="7"/>
       <c r="D27" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1938,12 +1918,10 @@
     </row>
     <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="33" t="s">
-        <v>192</v>
-      </c>
-      <c r="B28" s="33"/>
-      <c r="C28" s="33">
-        <v>13735</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
       <c r="D28" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1951,12 +1929,10 @@
     </row>
     <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="33" t="s">
-        <v>193</v>
-      </c>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7">
-        <v>14417</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="B29" s="33"/>
+      <c r="C29" s="33"/>
       <c r="D29" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1964,38 +1940,32 @@
     </row>
     <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7">
-        <v>15063</v>
-      </c>
-      <c r="D30" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7">
-        <v>15660</v>
-      </c>
-      <c r="D31" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
-        <v>196</v>
-      </c>
       <c r="B32" s="7"/>
-      <c r="C32" s="7">
-        <v>16305</v>
-      </c>
+      <c r="C32" s="7"/>
       <c r="D32" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2003,12 +1973,10 @@
     </row>
     <row r="33" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B33" s="7"/>
-      <c r="C33" s="7">
-        <v>16830</v>
-      </c>
+      <c r="C33" s="7"/>
       <c r="D33" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2016,12 +1984,10 @@
     </row>
     <row r="34" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B34" s="7"/>
-      <c r="C34" s="7">
-        <v>17476</v>
-      </c>
+      <c r="C34" s="7"/>
       <c r="D34" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2029,12 +1995,10 @@
     </row>
     <row r="35" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B35" s="7"/>
-      <c r="C35" s="7">
-        <v>18217</v>
-      </c>
+      <c r="C35" s="7"/>
       <c r="D35" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2042,26 +2006,21 @@
     </row>
     <row r="36" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B36" s="7"/>
-      <c r="C36" s="7">
-        <v>18855</v>
-      </c>
+      <c r="C36" s="7"/>
       <c r="D36" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E36" s="7"/>
     </row>
     <row r="37" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B37" s="7"/>
-      <c r="C37" s="7">
-        <v>19222</v>
-      </c>
+      <c r="C37" s="7"/>
       <c r="D37" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2070,38 +2029,33 @@
     </row>
     <row r="38" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="E38" s="7"/>
+    </row>
+    <row r="39" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7">
-        <v>19867</v>
-      </c>
-      <c r="D38" s="3" t="str">
-        <f t="shared" ref="D38:D69" si="2">IF(C38&lt;&gt;"",IF(B38&lt;&gt;"",C38-B38,"-"), "-")</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="33" t="s">
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="3" t="str">
+        <f t="shared" ref="D39:D70" si="2">IF(C39&lt;&gt;"",IF(B39&lt;&gt;"",C39-B39,"-"), "-")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40" s="33" t="s">
         <v>232</v>
       </c>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7">
-        <v>20034</v>
-      </c>
-      <c r="D39" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="7" t="s">
-        <v>202</v>
-      </c>
       <c r="B40" s="7"/>
-      <c r="C40" s="7">
-        <v>20738</v>
-      </c>
+      <c r="C40" s="7"/>
       <c r="D40" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2109,12 +2063,10 @@
     </row>
     <row r="41" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B41" s="7"/>
-      <c r="C41" s="7">
-        <v>21383</v>
-      </c>
+      <c r="C41" s="7"/>
       <c r="D41" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2122,12 +2074,10 @@
     </row>
     <row r="42" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8">
-        <v>22330</v>
-      </c>
+        <v>203</v>
+      </c>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
       <c r="D42" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2135,12 +2085,10 @@
     </row>
     <row r="43" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="B43" s="33"/>
-      <c r="C43" s="33">
-        <v>22994</v>
-      </c>
+        <v>204</v>
+      </c>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
       <c r="D43" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2148,12 +2096,10 @@
     </row>
     <row r="44" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="B44" s="7"/>
-      <c r="C44" s="7">
-        <v>23293</v>
-      </c>
+        <v>205</v>
+      </c>
+      <c r="B44" s="33"/>
+      <c r="C44" s="33"/>
       <c r="D44" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2161,12 +2107,10 @@
     </row>
     <row r="45" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B45" s="7"/>
-      <c r="C45" s="7">
-        <v>23953</v>
-      </c>
+      <c r="C45" s="7"/>
       <c r="D45" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2174,12 +2118,10 @@
     </row>
     <row r="46" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B46" s="7"/>
-      <c r="C46" s="7">
-        <v>24530</v>
-      </c>
+      <c r="C46" s="7"/>
       <c r="D46" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2187,12 +2129,10 @@
     </row>
     <row r="47" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B47" s="7"/>
-      <c r="C47" s="7">
-        <v>25190</v>
-      </c>
+      <c r="C47" s="7"/>
       <c r="D47" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2200,12 +2140,10 @@
     </row>
     <row r="48" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B48" s="7"/>
-      <c r="C48" s="7">
-        <v>26022</v>
-      </c>
+      <c r="C48" s="7"/>
       <c r="D48" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2213,12 +2151,10 @@
     </row>
     <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B49" s="7"/>
-      <c r="C49" s="7">
-        <v>26681</v>
-      </c>
+      <c r="C49" s="7"/>
       <c r="D49" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2226,12 +2162,10 @@
     </row>
     <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B50" s="7"/>
-      <c r="C50" s="7">
-        <v>27241</v>
-      </c>
+      <c r="C50" s="7"/>
       <c r="D50" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2239,12 +2173,10 @@
     </row>
     <row r="51" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B51" s="7"/>
-      <c r="C51" s="7">
-        <v>27889</v>
-      </c>
+      <c r="C51" s="7"/>
       <c r="D51" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2252,12 +2184,10 @@
     </row>
     <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B52" s="7"/>
-      <c r="C52" s="7">
-        <v>28945</v>
-      </c>
+      <c r="C52" s="7"/>
       <c r="D52" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2265,12 +2195,10 @@
     </row>
     <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B53" s="7"/>
-      <c r="C53" s="7">
-        <v>29444</v>
-      </c>
+      <c r="C53" s="7"/>
       <c r="D53" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2278,12 +2206,10 @@
     </row>
     <row r="54" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B54" s="7"/>
-      <c r="C54" s="7">
-        <v>29868</v>
-      </c>
+      <c r="C54" s="7"/>
       <c r="D54" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2291,12 +2217,10 @@
     </row>
     <row r="55" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B55" s="7"/>
-      <c r="C55" s="7">
-        <v>30507</v>
-      </c>
+      <c r="C55" s="7"/>
       <c r="D55" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2304,12 +2228,10 @@
     </row>
     <row r="56" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B56" s="7"/>
-      <c r="C56" s="7">
-        <v>31061</v>
-      </c>
+      <c r="C56" s="7"/>
       <c r="D56" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2317,12 +2239,10 @@
     </row>
     <row r="57" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B57" s="7"/>
-      <c r="C57" s="7">
-        <v>31706</v>
-      </c>
+      <c r="C57" s="7"/>
       <c r="D57" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2330,12 +2250,10 @@
     </row>
     <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B58" s="7"/>
-      <c r="C58" s="7">
-        <v>32622</v>
-      </c>
+      <c r="C58" s="7"/>
       <c r="D58" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2343,12 +2261,10 @@
     </row>
     <row r="59" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B59" s="7"/>
-      <c r="C59" s="7">
-        <v>33269</v>
-      </c>
+      <c r="C59" s="7"/>
       <c r="D59" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2356,12 +2272,10 @@
     </row>
     <row r="60" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B60" s="7"/>
-      <c r="C60" s="7">
-        <v>34177</v>
-      </c>
+      <c r="C60" s="7"/>
       <c r="D60" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2369,12 +2283,10 @@
     </row>
     <row r="61" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B61" s="7"/>
-      <c r="C61" s="7">
-        <v>34821</v>
-      </c>
+      <c r="C61" s="7"/>
       <c r="D61" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2382,12 +2294,10 @@
     </row>
     <row r="62" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B62" s="7"/>
-      <c r="C62" s="7">
-        <v>35636</v>
-      </c>
+      <c r="C62" s="7"/>
       <c r="D62" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2395,12 +2305,10 @@
     </row>
     <row r="63" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B63" s="7"/>
-      <c r="C63" s="7">
-        <v>36237</v>
-      </c>
+      <c r="C63" s="7"/>
       <c r="D63" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2408,12 +2316,10 @@
     </row>
     <row r="64" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>27</v>
+        <v>225</v>
       </c>
       <c r="B64" s="7"/>
-      <c r="C64" s="7">
-        <v>37327</v>
-      </c>
+      <c r="C64" s="7"/>
       <c r="D64" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2421,25 +2327,21 @@
     </row>
     <row r="65" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>226</v>
+        <v>27</v>
       </c>
       <c r="B65" s="7"/>
-      <c r="C65" s="7">
-        <v>37819</v>
-      </c>
+      <c r="C65" s="7"/>
       <c r="D65" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A66" s="34" t="s">
-        <v>234</v>
+      <c r="A66" s="7" t="s">
+        <v>226</v>
       </c>
       <c r="B66" s="7"/>
-      <c r="C66" s="7">
-        <v>38071</v>
-      </c>
+      <c r="C66" s="7"/>
       <c r="D66" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2447,12 +2349,10 @@
     </row>
     <row r="67" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="34" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B67" s="7"/>
-      <c r="C67" s="7">
-        <v>38132</v>
-      </c>
+      <c r="C67" s="7"/>
       <c r="D67" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2460,25 +2360,21 @@
     </row>
     <row r="68" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="34" t="s">
-        <v>150</v>
+        <v>233</v>
       </c>
       <c r="B68" s="7"/>
-      <c r="C68" s="7">
-        <v>38145</v>
-      </c>
+      <c r="C68" s="7"/>
       <c r="D68" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A69" s="7" t="s">
-        <v>227</v>
+      <c r="A69" s="34" t="s">
+        <v>150</v>
       </c>
       <c r="B69" s="7"/>
-      <c r="C69" s="7">
-        <v>38527</v>
-      </c>
+      <c r="C69" s="7"/>
       <c r="D69" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2486,38 +2382,32 @@
     </row>
     <row r="70" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B70" s="7"/>
-      <c r="C70" s="7">
-        <v>39151</v>
-      </c>
+      <c r="C70" s="7"/>
       <c r="D70" s="3" t="str">
-        <f t="shared" ref="D70:D101" si="3">IF(C70&lt;&gt;"",IF(B70&lt;&gt;"",C70-B70,"-"), "-")</f>
+        <f t="shared" si="2"/>
         <v>-</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="B71" s="9"/>
-      <c r="C71" s="9">
-        <v>39334</v>
-      </c>
+        <v>228</v>
+      </c>
+      <c r="B71" s="7"/>
+      <c r="C71" s="7"/>
       <c r="D71" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="D71:D77" si="3">IF(C71&lt;&gt;"",IF(B71&lt;&gt;"",C71-B71,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="B72" s="7"/>
-      <c r="C72" s="7">
-        <v>39973</v>
-      </c>
+        <v>229</v>
+      </c>
+      <c r="B72" s="9"/>
+      <c r="C72" s="9"/>
       <c r="D72" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
@@ -2525,12 +2415,10 @@
     </row>
     <row r="73" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="B73" s="9"/>
-      <c r="C73" s="9">
-        <v>40494</v>
-      </c>
+        <v>230</v>
+      </c>
+      <c r="B73" s="7"/>
+      <c r="C73" s="7"/>
       <c r="D73" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
@@ -2538,12 +2426,10 @@
     </row>
     <row r="74" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="B74" s="7"/>
-      <c r="C74" s="7">
-        <v>41139</v>
-      </c>
+        <v>231</v>
+      </c>
+      <c r="B74" s="9"/>
+      <c r="C74" s="9"/>
       <c r="D74" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
@@ -2551,25 +2437,21 @@
     </row>
     <row r="75" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B75" s="7"/>
-      <c r="C75" s="7">
-        <v>41742</v>
-      </c>
+      <c r="C75" s="7"/>
       <c r="D75" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A76" s="5" t="s">
-        <v>10</v>
+      <c r="A76" s="7" t="s">
+        <v>124</v>
       </c>
       <c r="B76" s="7"/>
-      <c r="C76" s="7">
-        <v>42387</v>
-      </c>
+      <c r="C76" s="7"/>
       <c r="D76" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
@@ -2577,38 +2459,32 @@
     </row>
     <row r="77" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="B77" s="7"/>
-      <c r="C77" s="7">
-        <v>43033</v>
-      </c>
+      <c r="C77" s="7"/>
       <c r="D77" s="3" t="str">
-        <f t="shared" ref="D77:D145" si="4">IF(C77&lt;&gt;"",IF(B77&lt;&gt;"",C77-B77,"-"), "-")</f>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="B78" s="7"/>
-      <c r="C78" s="7">
-        <v>43693</v>
-      </c>
+      <c r="C78" s="7"/>
       <c r="D78" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="D78:D146" si="4">IF(C78&lt;&gt;"",IF(B78&lt;&gt;"",C78-B78,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B79" s="7"/>
-      <c r="C79" s="7">
-        <v>44329</v>
-      </c>
+      <c r="C79" s="7"/>
       <c r="D79" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
@@ -2616,12 +2492,10 @@
     </row>
     <row r="80" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="B80" s="7"/>
-      <c r="C80" s="7">
-        <v>44988</v>
-      </c>
+      <c r="C80" s="7"/>
       <c r="D80" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
@@ -2629,12 +2503,10 @@
     </row>
     <row r="81" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="B81" s="7"/>
-      <c r="C81" s="7">
-        <v>45587</v>
-      </c>
+      <c r="C81" s="7"/>
       <c r="D81" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
@@ -2642,25 +2514,21 @@
     </row>
     <row r="82" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="B82" s="7"/>
-      <c r="C82" s="7">
-        <v>46248</v>
-      </c>
+      <c r="C82" s="7"/>
       <c r="D82" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A83" s="7" t="s">
-        <v>47</v>
+      <c r="A83" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="B83" s="7"/>
-      <c r="C83" s="7">
-        <v>47029</v>
-      </c>
+      <c r="C83" s="7"/>
       <c r="D83" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
@@ -2668,51 +2536,43 @@
     </row>
     <row r="84" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B84" s="7"/>
-      <c r="C84" s="7">
-        <v>47527</v>
-      </c>
+      <c r="C84" s="7"/>
       <c r="D84" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A85" s="34" t="s">
-        <v>235</v>
+      <c r="A85" s="7" t="s">
+        <v>48</v>
       </c>
       <c r="B85" s="7"/>
-      <c r="C85" s="7">
-        <v>48010</v>
-      </c>
+      <c r="C85" s="7"/>
       <c r="D85" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A86" s="7" t="s">
-        <v>33</v>
+      <c r="A86" s="34" t="s">
+        <v>235</v>
       </c>
       <c r="B86" s="7"/>
-      <c r="C86" s="7">
-        <v>48393</v>
-      </c>
+      <c r="C86" s="7"/>
       <c r="D86" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A87" s="5" t="s">
-        <v>14</v>
+      <c r="A87" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="B87" s="7"/>
-      <c r="C87" s="7">
-        <v>49053</v>
-      </c>
+      <c r="C87" s="7"/>
       <c r="D87" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
@@ -2720,12 +2580,10 @@
     </row>
     <row r="88" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="B88" s="7"/>
-      <c r="C88" s="7">
-        <v>49311</v>
-      </c>
+      <c r="C88" s="7"/>
       <c r="D88" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
@@ -2733,12 +2591,10 @@
     </row>
     <row r="89" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="B89" s="7"/>
-      <c r="C89" s="7">
-        <v>49911</v>
-      </c>
+      <c r="C89" s="7"/>
       <c r="D89" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
@@ -2746,12 +2602,10 @@
     </row>
     <row r="90" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="B90" s="7"/>
-      <c r="C90" s="7">
-        <v>50889</v>
-      </c>
+      <c r="C90" s="7"/>
       <c r="D90" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
@@ -2759,12 +2613,10 @@
     </row>
     <row r="91" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="B91" s="7"/>
-      <c r="C91" s="7">
-        <v>51535</v>
-      </c>
+      <c r="C91" s="7"/>
       <c r="D91" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
@@ -2772,12 +2624,10 @@
     </row>
     <row r="92" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="B92" s="7"/>
-      <c r="C92" s="7">
-        <v>52312</v>
-      </c>
+      <c r="C92" s="7"/>
       <c r="D92" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
@@ -2785,12 +2635,10 @@
     </row>
     <row r="93" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="B93" s="7"/>
-      <c r="C93" s="7">
-        <v>52934</v>
-      </c>
+      <c r="C93" s="7"/>
       <c r="D93" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
@@ -2798,12 +2646,10 @@
     </row>
     <row r="94" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="B94" s="7"/>
-      <c r="C94" s="7">
-        <v>53936</v>
-      </c>
+      <c r="C94" s="7"/>
       <c r="D94" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
@@ -2811,12 +2657,10 @@
     </row>
     <row r="95" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="B95" s="7"/>
-      <c r="C95" s="7">
-        <v>54526</v>
-      </c>
+      <c r="C95" s="7"/>
       <c r="D95" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
@@ -2824,12 +2668,10 @@
     </row>
     <row r="96" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="B96" s="7"/>
-      <c r="C96" s="7">
-        <v>54878</v>
-      </c>
+      <c r="C96" s="7"/>
       <c r="D96" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
@@ -2837,12 +2679,10 @@
     </row>
     <row r="97" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="B97" s="7"/>
-      <c r="C97" s="7">
-        <v>55524</v>
-      </c>
+      <c r="C97" s="7"/>
       <c r="D97" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
@@ -2850,12 +2690,10 @@
     </row>
     <row r="98" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="B98" s="7"/>
-      <c r="C98" s="7">
-        <v>56204</v>
-      </c>
+      <c r="C98" s="7"/>
       <c r="D98" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
@@ -2863,12 +2701,10 @@
     </row>
     <row r="99" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="B99" s="7"/>
-      <c r="C99" s="7">
-        <v>56804</v>
-      </c>
+      <c r="C99" s="7"/>
       <c r="D99" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
@@ -2876,12 +2712,10 @@
     </row>
     <row r="100" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="B100" s="7"/>
-      <c r="C100" s="7">
-        <v>57359</v>
-      </c>
+      <c r="C100" s="7"/>
       <c r="D100" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
@@ -2889,12 +2723,10 @@
     </row>
     <row r="101" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="B101" s="7"/>
-      <c r="C101" s="7">
-        <v>57995</v>
-      </c>
+      <c r="C101" s="7"/>
       <c r="D101" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
@@ -2902,12 +2734,10 @@
     </row>
     <row r="102" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="B102" s="7"/>
-      <c r="C102" s="7">
-        <v>58575</v>
-      </c>
+      <c r="C102" s="7"/>
       <c r="D102" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
@@ -2915,12 +2745,10 @@
     </row>
     <row r="103" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="B103" s="7"/>
-      <c r="C103" s="7">
-        <v>59227</v>
-      </c>
+      <c r="C103" s="7"/>
       <c r="D103" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
@@ -2928,12 +2756,10 @@
     </row>
     <row r="104" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B104" s="10"/>
-      <c r="C104" s="10">
-        <v>60018</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="B104" s="7"/>
+      <c r="C104" s="7"/>
       <c r="D104" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
@@ -2941,38 +2767,32 @@
     </row>
     <row r="105" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B105" s="7"/>
-      <c r="C105" s="7">
-        <v>60663</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="B105" s="10"/>
+      <c r="C105" s="10"/>
       <c r="D105" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A106" s="35" t="s">
-        <v>127</v>
+      <c r="A106" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="B106" s="7"/>
-      <c r="C106" s="7">
-        <v>60822</v>
-      </c>
+      <c r="C106" s="7"/>
       <c r="D106" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A107" s="5" t="s">
-        <v>43</v>
+      <c r="A107" s="35" t="s">
+        <v>127</v>
       </c>
       <c r="B107" s="7"/>
-      <c r="C107" s="7">
-        <v>61231</v>
-      </c>
+      <c r="C107" s="7"/>
       <c r="D107" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
@@ -2980,12 +2800,10 @@
     </row>
     <row r="108" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="B108" s="7"/>
-      <c r="C108" s="7">
-        <v>61891</v>
-      </c>
+      <c r="C108" s="7"/>
       <c r="D108" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
@@ -2993,12 +2811,10 @@
     </row>
     <row r="109" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="B109" s="7"/>
-      <c r="C109" s="7">
-        <v>62598</v>
-      </c>
+      <c r="C109" s="7"/>
       <c r="D109" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
@@ -3006,56 +2822,48 @@
     </row>
     <row r="110" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="B110" s="7"/>
-      <c r="C110" s="7">
-        <v>63243</v>
-      </c>
+      <c r="C110" s="7"/>
       <c r="D110" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A111" s="5"/>
+      <c r="A111" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="B111" s="7"/>
-      <c r="C111" s="7">
-        <v>63497</v>
-      </c>
-      <c r="D111" s="3"/>
+      <c r="C111" s="7"/>
+      <c r="D111" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="112" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A112" s="5"/>
       <c r="B112" s="7"/>
-      <c r="C112" s="7">
-        <v>63552</v>
-      </c>
+      <c r="C112" s="7"/>
       <c r="D112" s="3"/>
     </row>
     <row r="113" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A113" s="5"/>
       <c r="B113" s="7"/>
-      <c r="C113" s="7">
-        <v>63603</v>
-      </c>
+      <c r="C113" s="7"/>
       <c r="D113" s="3"/>
     </row>
     <row r="114" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A114" s="5" t="s">
+      <c r="A114" s="5"/>
+      <c r="B114" s="7"/>
+      <c r="C114" s="7"/>
+      <c r="D114" s="3"/>
+    </row>
+    <row r="115" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A115" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B114" s="7"/>
-      <c r="C114" s="7">
-        <v>63782</v>
-      </c>
-      <c r="D114" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A115" s="7"/>
       <c r="B115" s="7"/>
       <c r="C115" s="7"/>
       <c r="D115" s="3" t="str">
@@ -3338,7 +3146,7 @@
       <c r="B146" s="7"/>
       <c r="C146" s="7"/>
       <c r="D146" s="3" t="str">
-        <f t="shared" ref="D146:D150" si="5">IF(C146&lt;&gt;"",IF(B146&lt;&gt;"",C146-B146,"-"), "-")</f>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
     </row>
@@ -3347,7 +3155,7 @@
       <c r="B147" s="7"/>
       <c r="C147" s="7"/>
       <c r="D147" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="D147:D151" si="5">IF(C147&lt;&gt;"",IF(B147&lt;&gt;"",C147-B147,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
@@ -3383,7 +3191,7 @@
       <c r="B151" s="7"/>
       <c r="C151" s="7"/>
       <c r="D151" s="3" t="str">
-        <f t="shared" ref="D151:D152" si="6">IF(C151&lt;&gt;"",IF(B151&lt;&gt;"",B151-C151,"-"), "-")</f>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
     </row>
@@ -3392,7 +3200,7 @@
       <c r="B152" s="7"/>
       <c r="C152" s="7"/>
       <c r="D152" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="D152:D153" si="6">IF(C152&lt;&gt;"",IF(B152&lt;&gt;"",B152-C152,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
@@ -3400,6 +3208,10 @@
       <c r="A153" s="7"/>
       <c r="B153" s="7"/>
       <c r="C153" s="7"/>
+      <c r="D153" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="154" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A154" s="7"/>
@@ -3407,6 +3219,7 @@
       <c r="C154" s="7"/>
     </row>
     <row r="155" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A155" s="7"/>
       <c r="B155" s="7"/>
       <c r="C155" s="7"/>
     </row>
@@ -3953,6 +3766,10 @@
     <row r="291" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B291" s="7"/>
       <c r="C291" s="7"/>
+    </row>
+    <row r="292" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B292" s="7"/>
+      <c r="C292" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13967,7 +13784,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="17" type="noConversion"/>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0" right="0" top="0.39410000000000006" bottom="0.39410000000000006" header="0" footer="0"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
@@ -14002,10 +13819,10 @@
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
       <c r="J1" s="15"/>
-      <c r="K1" s="36" t="s">
+      <c r="K1" s="37" t="s">
         <v>158</v>
       </c>
-      <c r="L1" s="37"/>
+      <c r="L1" s="38"/>
     </row>
     <row r="2" spans="1:12" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
@@ -15857,13 +15674,13 @@
       <c r="G53" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="H53" s="38" t="s">
+      <c r="H53" s="39" t="s">
         <v>165</v>
       </c>
-      <c r="I53" s="39"/>
-      <c r="J53" s="39"/>
-      <c r="K53" s="39"/>
-      <c r="L53" s="40"/>
+      <c r="I53" s="40"/>
+      <c r="J53" s="40"/>
+      <c r="K53" s="40"/>
+      <c r="L53" s="41"/>
     </row>
     <row r="54" spans="1:12" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="11"/>
@@ -15885,11 +15702,11 @@
       <c r="G54" s="27">
         <v>31536</v>
       </c>
-      <c r="H54" s="41"/>
-      <c r="I54" s="42"/>
-      <c r="J54" s="42"/>
-      <c r="K54" s="42"/>
-      <c r="L54" s="43"/>
+      <c r="H54" s="42"/>
+      <c r="I54" s="43"/>
+      <c r="J54" s="43"/>
+      <c r="K54" s="43"/>
+      <c r="L54" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
lv 2 scroll skip
</commit_message>
<xml_diff>
--- a/LodeRunner/compare.xlsx
+++ b/LodeRunner/compare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\LodeRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C7F00D3-00C6-48BA-BE05-ABEB53498FE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8701FAA3-5727-4EE9-844E-1BA6188581BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="50280" yWindow="3255" windowWidth="7305" windowHeight="12990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1578,7 +1578,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1695,27 +1695,29 @@
         <v>242</v>
       </c>
       <c r="B8" s="7">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="C8" s="7">
         <v>1049</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" si="0"/>
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="45" t="s">
         <v>243</v>
       </c>
-      <c r="B9" s="7"/>
+      <c r="B9" s="7">
+        <v>1101</v>
+      </c>
       <c r="C9" s="7">
         <v>1704</v>
       </c>
-      <c r="D9" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D9" s="3">
+        <f t="shared" si="0"/>
+        <v>603</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
lode runner - lua stuff
</commit_message>
<xml_diff>
--- a/LodeRunner/compare.xlsx
+++ b/LodeRunner/compare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\LodeRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8701FAA3-5727-4EE9-844E-1BA6188581BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26ACC482-5121-48F0-86A6-78FE374CC3FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="50280" yWindow="3255" windowWidth="7305" windowHeight="12990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="246">
   <si>
     <t>Place</t>
   </si>
@@ -767,6 +767,12 @@
   </si>
   <si>
     <t>02 1st move</t>
+  </si>
+  <si>
+    <t>8 frames luck manip</t>
+  </si>
+  <si>
+    <t>start 2 tile dig</t>
   </si>
 </sst>
 </file>
@@ -1574,11 +1580,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB48F502-AA0A-4BF9-ABA2-AA87E3F2B5E4}">
-  <dimension ref="A1:E292"/>
+  <dimension ref="A1:E293"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1586,9 +1592,10 @@
     <col min="1" max="1" width="15.125" customWidth="1"/>
     <col min="2" max="3" width="8.75" customWidth="1"/>
     <col min="4" max="4" width="6.625" customWidth="1"/>
+    <col min="5" max="5" width="17.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1602,7 +1609,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="36" t="s">
         <v>237</v>
       </c>
@@ -1613,11 +1620,11 @@
         <v>426</v>
       </c>
       <c r="D2" s="3">
-        <f t="shared" ref="D2:D38" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
+        <f t="shared" ref="D2:D39" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="36" t="s">
         <v>238</v>
       </c>
@@ -1632,7 +1639,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="36" t="s">
         <v>239</v>
       </c>
@@ -1647,7 +1654,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="36" t="s">
         <v>240</v>
       </c>
@@ -1662,7 +1669,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="36" t="s">
         <v>241</v>
       </c>
@@ -1677,7 +1684,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="36"/>
       <c r="B7" s="2">
         <v>812</v>
@@ -1690,7 +1697,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
         <v>242</v>
       </c>
@@ -1705,35 +1712,42 @@
         <v>295</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="45" t="s">
         <v>243</v>
       </c>
       <c r="B9" s="7">
-        <v>1101</v>
+        <v>1109</v>
       </c>
       <c r="C9" s="7">
         <v>1704</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" si="0"/>
-        <v>603</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="33" t="s">
+        <v>595</v>
+      </c>
+      <c r="E9" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="45" t="s">
+        <v>245</v>
+      </c>
+      <c r="B10" s="7">
+        <v>1241</v>
+      </c>
+      <c r="C10" s="7">
+        <v>1830</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="0"/>
+        <v>589</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="33" t="s">
         <v>173</v>
-      </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="33" t="s">
-        <v>174</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -1742,9 +1756,9 @@
         <v>-</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="33" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -1753,9 +1767,9 @@
         <v>-</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -1764,9 +1778,9 @@
         <v>-</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -1775,9 +1789,9 @@
         <v>-</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -1786,9 +1800,9 @@
         <v>-</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="33" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -1799,7 +1813,7 @@
     </row>
     <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="33" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
@@ -1810,7 +1824,7 @@
     </row>
     <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="33" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -1821,7 +1835,7 @@
     </row>
     <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="33" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -1832,7 +1846,7 @@
     </row>
     <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -1843,7 +1857,7 @@
     </row>
     <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="33" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
@@ -1854,7 +1868,7 @@
     </row>
     <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="33" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -1865,7 +1879,7 @@
     </row>
     <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="33" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -1876,7 +1890,7 @@
     </row>
     <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="33" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -1887,7 +1901,7 @@
     </row>
     <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -1898,7 +1912,7 @@
     </row>
     <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="33" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
@@ -1909,7 +1923,7 @@
     </row>
     <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="33" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
@@ -1920,7 +1934,7 @@
     </row>
     <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="33" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
@@ -1931,10 +1945,10 @@
     </row>
     <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="33" t="s">
-        <v>192</v>
-      </c>
-      <c r="B29" s="33"/>
-      <c r="C29" s="33"/>
+        <v>191</v>
+      </c>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
       <c r="D29" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1942,10 +1956,10 @@
     </row>
     <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="33" t="s">
-        <v>193</v>
-      </c>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
+        <v>192</v>
+      </c>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
       <c r="D30" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1953,7 +1967,7 @@
     </row>
     <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="33" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
@@ -1963,8 +1977,8 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
-        <v>195</v>
+      <c r="A32" s="33" t="s">
+        <v>194</v>
       </c>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
@@ -1974,8 +1988,8 @@
       </c>
     </row>
     <row r="33" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
-        <v>196</v>
+      <c r="A33" s="8" t="s">
+        <v>195</v>
       </c>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
@@ -1986,7 +2000,7 @@
     </row>
     <row r="34" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
@@ -1997,7 +2011,7 @@
     </row>
     <row r="35" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
@@ -2008,7 +2022,7 @@
     </row>
     <row r="36" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
@@ -2019,7 +2033,7 @@
     </row>
     <row r="37" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
@@ -2027,11 +2041,10 @@
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E37" s="7"/>
     </row>
     <row r="38" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
@@ -2043,29 +2056,30 @@
     </row>
     <row r="39" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
       <c r="D39" s="3" t="str">
-        <f t="shared" ref="D39:D70" si="2">IF(C39&lt;&gt;"",IF(B39&lt;&gt;"",C39-B39,"-"), "-")</f>
-        <v>-</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="E39" s="7"/>
     </row>
     <row r="40" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="33" t="s">
-        <v>232</v>
+      <c r="A40" s="7" t="s">
+        <v>201</v>
       </c>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
       <c r="D40" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="D40:D71" si="2">IF(C40&lt;&gt;"",IF(B40&lt;&gt;"",C40-B40,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="7" t="s">
-        <v>202</v>
+      <c r="A41" s="33" t="s">
+        <v>232</v>
       </c>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
@@ -2076,7 +2090,7 @@
     </row>
     <row r="42" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
@@ -2087,10 +2101,10 @@
     </row>
     <row r="43" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="B43" s="8"/>
-      <c r="C43" s="8"/>
+        <v>203</v>
+      </c>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
       <c r="D43" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2098,10 +2112,10 @@
     </row>
     <row r="44" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="B44" s="33"/>
-      <c r="C44" s="33"/>
+        <v>204</v>
+      </c>
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
       <c r="D44" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2109,10 +2123,10 @@
     </row>
     <row r="45" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="B45" s="7"/>
-      <c r="C45" s="7"/>
+        <v>205</v>
+      </c>
+      <c r="B45" s="33"/>
+      <c r="C45" s="33"/>
       <c r="D45" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2120,7 +2134,7 @@
     </row>
     <row r="46" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
@@ -2131,7 +2145,7 @@
     </row>
     <row r="47" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
@@ -2142,7 +2156,7 @@
     </row>
     <row r="48" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
@@ -2153,7 +2167,7 @@
     </row>
     <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
@@ -2164,7 +2178,7 @@
     </row>
     <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
@@ -2175,7 +2189,7 @@
     </row>
     <row r="51" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
@@ -2186,7 +2200,7 @@
     </row>
     <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
@@ -2197,7 +2211,7 @@
     </row>
     <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
@@ -2208,7 +2222,7 @@
     </row>
     <row r="54" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B54" s="7"/>
       <c r="C54" s="7"/>
@@ -2219,7 +2233,7 @@
     </row>
     <row r="55" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
@@ -2230,7 +2244,7 @@
     </row>
     <row r="56" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
@@ -2241,7 +2255,7 @@
     </row>
     <row r="57" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
@@ -2252,7 +2266,7 @@
     </row>
     <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B58" s="7"/>
       <c r="C58" s="7"/>
@@ -2263,7 +2277,7 @@
     </row>
     <row r="59" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B59" s="7"/>
       <c r="C59" s="7"/>
@@ -2274,7 +2288,7 @@
     </row>
     <row r="60" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
@@ -2285,7 +2299,7 @@
     </row>
     <row r="61" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
@@ -2296,7 +2310,7 @@
     </row>
     <row r="62" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
@@ -2307,7 +2321,7 @@
     </row>
     <row r="63" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
@@ -2318,7 +2332,7 @@
     </row>
     <row r="64" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
@@ -2329,7 +2343,7 @@
     </row>
     <row r="65" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>27</v>
+        <v>225</v>
       </c>
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
@@ -2340,7 +2354,7 @@
     </row>
     <row r="66" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>226</v>
+        <v>27</v>
       </c>
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
@@ -2350,8 +2364,8 @@
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A67" s="34" t="s">
-        <v>234</v>
+      <c r="A67" s="7" t="s">
+        <v>226</v>
       </c>
       <c r="B67" s="7"/>
       <c r="C67" s="7"/>
@@ -2362,7 +2376,7 @@
     </row>
     <row r="68" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="34" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B68" s="7"/>
       <c r="C68" s="7"/>
@@ -2373,7 +2387,7 @@
     </row>
     <row r="69" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="34" t="s">
-        <v>150</v>
+        <v>233</v>
       </c>
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
@@ -2383,8 +2397,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A70" s="7" t="s">
-        <v>227</v>
+      <c r="A70" s="34" t="s">
+        <v>150</v>
       </c>
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
@@ -2395,32 +2409,32 @@
     </row>
     <row r="71" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B71" s="7"/>
       <c r="C71" s="7"/>
       <c r="D71" s="3" t="str">
-        <f t="shared" ref="D71:D77" si="3">IF(C71&lt;&gt;"",IF(B71&lt;&gt;"",C71-B71,"-"), "-")</f>
+        <f t="shared" si="2"/>
         <v>-</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="B72" s="9"/>
-      <c r="C72" s="9"/>
+        <v>228</v>
+      </c>
+      <c r="B72" s="7"/>
+      <c r="C72" s="7"/>
       <c r="D72" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="D72:D78" si="3">IF(C72&lt;&gt;"",IF(B72&lt;&gt;"",C72-B72,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="B73" s="7"/>
-      <c r="C73" s="7"/>
+        <v>229</v>
+      </c>
+      <c r="B73" s="9"/>
+      <c r="C73" s="9"/>
       <c r="D73" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
@@ -2428,10 +2442,10 @@
     </row>
     <row r="74" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="B74" s="9"/>
-      <c r="C74" s="9"/>
+        <v>230</v>
+      </c>
+      <c r="B74" s="7"/>
+      <c r="C74" s="7"/>
       <c r="D74" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
@@ -2439,10 +2453,10 @@
     </row>
     <row r="75" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="B75" s="7"/>
-      <c r="C75" s="7"/>
+        <v>231</v>
+      </c>
+      <c r="B75" s="9"/>
+      <c r="C75" s="9"/>
       <c r="D75" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
@@ -2450,7 +2464,7 @@
     </row>
     <row r="76" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B76" s="7"/>
       <c r="C76" s="7"/>
@@ -2460,8 +2474,8 @@
       </c>
     </row>
     <row r="77" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A77" s="5" t="s">
-        <v>10</v>
+      <c r="A77" s="7" t="s">
+        <v>124</v>
       </c>
       <c r="B77" s="7"/>
       <c r="C77" s="7"/>
@@ -2472,29 +2486,29 @@
     </row>
     <row r="78" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="B78" s="7"/>
       <c r="C78" s="7"/>
       <c r="D78" s="3" t="str">
-        <f t="shared" ref="D78:D146" si="4">IF(C78&lt;&gt;"",IF(B78&lt;&gt;"",C78-B78,"-"), "-")</f>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="B79" s="7"/>
       <c r="C79" s="7"/>
       <c r="D79" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="D79:D147" si="4">IF(C79&lt;&gt;"",IF(B79&lt;&gt;"",C79-B79,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B80" s="7"/>
       <c r="C80" s="7"/>
@@ -2505,7 +2519,7 @@
     </row>
     <row r="81" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="B81" s="7"/>
       <c r="C81" s="7"/>
@@ -2516,7 +2530,7 @@
     </row>
     <row r="82" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="B82" s="7"/>
       <c r="C82" s="7"/>
@@ -2527,7 +2541,7 @@
     </row>
     <row r="83" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="B83" s="7"/>
       <c r="C83" s="7"/>
@@ -2537,8 +2551,8 @@
       </c>
     </row>
     <row r="84" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A84" s="7" t="s">
-        <v>47</v>
+      <c r="A84" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="B84" s="7"/>
       <c r="C84" s="7"/>
@@ -2549,7 +2563,7 @@
     </row>
     <row r="85" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B85" s="7"/>
       <c r="C85" s="7"/>
@@ -2559,8 +2573,8 @@
       </c>
     </row>
     <row r="86" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A86" s="34" t="s">
-        <v>235</v>
+      <c r="A86" s="7" t="s">
+        <v>48</v>
       </c>
       <c r="B86" s="7"/>
       <c r="C86" s="7"/>
@@ -2570,8 +2584,8 @@
       </c>
     </row>
     <row r="87" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A87" s="7" t="s">
-        <v>33</v>
+      <c r="A87" s="34" t="s">
+        <v>235</v>
       </c>
       <c r="B87" s="7"/>
       <c r="C87" s="7"/>
@@ -2581,8 +2595,8 @@
       </c>
     </row>
     <row r="88" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A88" s="5" t="s">
-        <v>14</v>
+      <c r="A88" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="B88" s="7"/>
       <c r="C88" s="7"/>
@@ -2593,7 +2607,7 @@
     </row>
     <row r="89" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="B89" s="7"/>
       <c r="C89" s="7"/>
@@ -2604,7 +2618,7 @@
     </row>
     <row r="90" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
@@ -2615,7 +2629,7 @@
     </row>
     <row r="91" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="B91" s="7"/>
       <c r="C91" s="7"/>
@@ -2626,7 +2640,7 @@
     </row>
     <row r="92" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="B92" s="7"/>
       <c r="C92" s="7"/>
@@ -2637,7 +2651,7 @@
     </row>
     <row r="93" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="B93" s="7"/>
       <c r="C93" s="7"/>
@@ -2648,7 +2662,7 @@
     </row>
     <row r="94" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="B94" s="7"/>
       <c r="C94" s="7"/>
@@ -2659,7 +2673,7 @@
     </row>
     <row r="95" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="B95" s="7"/>
       <c r="C95" s="7"/>
@@ -2670,7 +2684,7 @@
     </row>
     <row r="96" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="B96" s="7"/>
       <c r="C96" s="7"/>
@@ -2681,7 +2695,7 @@
     </row>
     <row r="97" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="B97" s="7"/>
       <c r="C97" s="7"/>
@@ -2692,7 +2706,7 @@
     </row>
     <row r="98" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="B98" s="7"/>
       <c r="C98" s="7"/>
@@ -2703,7 +2717,7 @@
     </row>
     <row r="99" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="B99" s="7"/>
       <c r="C99" s="7"/>
@@ -2714,7 +2728,7 @@
     </row>
     <row r="100" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="B100" s="7"/>
       <c r="C100" s="7"/>
@@ -2725,7 +2739,7 @@
     </row>
     <row r="101" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="B101" s="7"/>
       <c r="C101" s="7"/>
@@ -2736,7 +2750,7 @@
     </row>
     <row r="102" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="B102" s="7"/>
       <c r="C102" s="7"/>
@@ -2747,7 +2761,7 @@
     </row>
     <row r="103" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="B103" s="7"/>
       <c r="C103" s="7"/>
@@ -2758,7 +2772,7 @@
     </row>
     <row r="104" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="B104" s="7"/>
       <c r="C104" s="7"/>
@@ -2769,10 +2783,10 @@
     </row>
     <row r="105" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B105" s="10"/>
-      <c r="C105" s="10"/>
+        <v>22</v>
+      </c>
+      <c r="B105" s="7"/>
+      <c r="C105" s="7"/>
       <c r="D105" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
@@ -2780,18 +2794,18 @@
     </row>
     <row r="106" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B106" s="7"/>
-      <c r="C106" s="7"/>
+        <v>42</v>
+      </c>
+      <c r="B106" s="10"/>
+      <c r="C106" s="10"/>
       <c r="D106" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A107" s="35" t="s">
-        <v>127</v>
+      <c r="A107" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="B107" s="7"/>
       <c r="C107" s="7"/>
@@ -2801,8 +2815,8 @@
       </c>
     </row>
     <row r="108" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A108" s="5" t="s">
-        <v>43</v>
+      <c r="A108" s="35" t="s">
+        <v>127</v>
       </c>
       <c r="B108" s="7"/>
       <c r="C108" s="7"/>
@@ -2813,7 +2827,7 @@
     </row>
     <row r="109" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="B109" s="7"/>
       <c r="C109" s="7"/>
@@ -2824,7 +2838,7 @@
     </row>
     <row r="110" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="B110" s="7"/>
       <c r="C110" s="7"/>
@@ -2835,7 +2849,7 @@
     </row>
     <row r="111" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="B111" s="7"/>
       <c r="C111" s="7"/>
@@ -2845,10 +2859,15 @@
       </c>
     </row>
     <row r="112" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A112" s="5"/>
+      <c r="A112" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="B112" s="7"/>
       <c r="C112" s="7"/>
-      <c r="D112" s="3"/>
+      <c r="D112" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="113" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A113" s="5"/>
@@ -2863,18 +2882,15 @@
       <c r="D114" s="3"/>
     </row>
     <row r="115" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A115" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="A115" s="5"/>
       <c r="B115" s="7"/>
       <c r="C115" s="7"/>
-      <c r="D115" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v>-</v>
-      </c>
+      <c r="D115" s="3"/>
     </row>
     <row r="116" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A116" s="7"/>
+      <c r="A116" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="B116" s="7"/>
       <c r="C116" s="7"/>
       <c r="D116" s="3" t="str">
@@ -3157,7 +3173,7 @@
       <c r="B147" s="7"/>
       <c r="C147" s="7"/>
       <c r="D147" s="3" t="str">
-        <f t="shared" ref="D147:D151" si="5">IF(C147&lt;&gt;"",IF(B147&lt;&gt;"",C147-B147,"-"), "-")</f>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
     </row>
@@ -3166,7 +3182,7 @@
       <c r="B148" s="7"/>
       <c r="C148" s="7"/>
       <c r="D148" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="D148:D152" si="5">IF(C148&lt;&gt;"",IF(B148&lt;&gt;"",C148-B148,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
@@ -3202,7 +3218,7 @@
       <c r="B152" s="7"/>
       <c r="C152" s="7"/>
       <c r="D152" s="3" t="str">
-        <f t="shared" ref="D152:D153" si="6">IF(C152&lt;&gt;"",IF(B152&lt;&gt;"",B152-C152,"-"), "-")</f>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
     </row>
@@ -3211,7 +3227,7 @@
       <c r="B153" s="7"/>
       <c r="C153" s="7"/>
       <c r="D153" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="D153:D154" si="6">IF(C153&lt;&gt;"",IF(B153&lt;&gt;"",B153-C153,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
@@ -3219,6 +3235,10 @@
       <c r="A154" s="7"/>
       <c r="B154" s="7"/>
       <c r="C154" s="7"/>
+      <c r="D154" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="155" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A155" s="7"/>
@@ -3226,6 +3246,7 @@
       <c r="C155" s="7"/>
     </row>
     <row r="156" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A156" s="7"/>
       <c r="B156" s="7"/>
       <c r="C156" s="7"/>
     </row>
@@ -3772,6 +3793,10 @@
     <row r="292" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B292" s="7"/>
       <c r="C292" s="7"/>
+    </row>
+    <row r="293" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B293" s="7"/>
+      <c r="C293" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
lode runner - 3 levels done, 1182 frames ahead
</commit_message>
<xml_diff>
--- a/LodeRunner/compare.xlsx
+++ b/LodeRunner/compare.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\LodeRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26ACC482-5121-48F0-86A6-78FE374CC3FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38760631-5265-4ECA-9981-51912F764CE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="50280" yWindow="3255" windowWidth="7305" windowHeight="12990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="50865" yWindow="3795" windowWidth="7170" windowHeight="12990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V6" sheetId="7" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="253">
   <si>
     <t>Place</t>
   </si>
@@ -773,6 +773,27 @@
   </si>
   <si>
     <t>start 2 tile dig</t>
+  </si>
+  <si>
+    <t>03 1st move</t>
+  </si>
+  <si>
+    <t>gold = 5</t>
+  </si>
+  <si>
+    <t>gold = 1</t>
+  </si>
+  <si>
+    <t>gold = 2</t>
+  </si>
+  <si>
+    <t>gold = 0</t>
+  </si>
+  <si>
+    <t>03 end</t>
+  </si>
+  <si>
+    <t>04 1st move</t>
   </si>
 </sst>
 </file>
@@ -1580,11 +1601,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB48F502-AA0A-4BF9-ABA2-AA87E3F2B5E4}">
-  <dimension ref="A1:E293"/>
+  <dimension ref="A1:E294"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1620,7 +1641,7 @@
         <v>426</v>
       </c>
       <c r="D2" s="3">
-        <f t="shared" ref="D2:D39" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
+        <f t="shared" ref="D2:D40" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
         <v>1</v>
       </c>
     </row>
@@ -1749,105 +1770,139 @@
       <c r="A11" s="33" t="s">
         <v>173</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="B11" s="7">
+        <v>1601</v>
+      </c>
+      <c r="C11" s="7">
+        <v>2182</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="0"/>
+        <v>581</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="33" t="s">
-        <v>174</v>
-      </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A12" s="45" t="s">
+        <v>246</v>
+      </c>
+      <c r="B12" s="7">
+        <v>1952</v>
+      </c>
+      <c r="C12" s="7">
+        <v>2837</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" si="0"/>
+        <v>885</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="33" t="s">
-        <v>175</v>
-      </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A13" s="45" t="s">
+        <v>247</v>
+      </c>
+      <c r="B13" s="7">
+        <v>2059</v>
+      </c>
+      <c r="C13" s="45">
+        <v>2943</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" si="0"/>
+        <v>884</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="33" t="s">
-        <v>176</v>
-      </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A14" s="45" t="s">
+        <v>127</v>
+      </c>
+      <c r="B14" s="7">
+        <v>2144</v>
+      </c>
+      <c r="C14" s="7">
+        <v>3028</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" si="0"/>
+        <v>884</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="33" t="s">
-        <v>177</v>
-      </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A15" s="45" t="s">
+        <v>249</v>
+      </c>
+      <c r="B15" s="7">
+        <v>2192</v>
+      </c>
+      <c r="C15" s="7">
+        <v>3076</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="0"/>
+        <v>884</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="33" t="s">
-        <v>178</v>
-      </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A16" s="45" t="s">
+        <v>248</v>
+      </c>
+      <c r="B16" s="7">
+        <v>2244</v>
+      </c>
+      <c r="C16" s="7">
+        <v>3124</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" si="0"/>
+        <v>880</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="33" t="s">
-        <v>179</v>
-      </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A17" s="45" t="s">
+        <v>250</v>
+      </c>
+      <c r="B17" s="7">
+        <v>2265</v>
+      </c>
+      <c r="C17" s="7">
+        <v>3146</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" si="0"/>
+        <v>881</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="33" t="s">
-        <v>180</v>
-      </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A18" s="45" t="s">
+        <v>251</v>
+      </c>
+      <c r="B18" s="7">
+        <v>2370</v>
+      </c>
+      <c r="C18" s="7">
+        <v>3248</v>
+      </c>
+      <c r="D18" s="3">
+        <f t="shared" si="0"/>
+        <v>878</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="33" t="s">
-        <v>181</v>
-      </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A19" s="45" t="s">
+        <v>252</v>
+      </c>
+      <c r="B19" s="7">
+        <v>2720</v>
+      </c>
+      <c r="C19" s="7">
+        <v>3902</v>
+      </c>
+      <c r="D19" s="3">
+        <f t="shared" si="0"/>
+        <v>1182</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="33" t="s">
-        <v>182</v>
-      </c>
+      <c r="A20" s="33"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="3" t="str">
@@ -1856,9 +1911,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="33" t="s">
-        <v>183</v>
-      </c>
+      <c r="A21" s="33"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="3" t="str">
@@ -1867,9 +1920,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="33" t="s">
-        <v>184</v>
-      </c>
+      <c r="A22" s="33"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="3" t="str">
@@ -1878,9 +1929,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="33" t="s">
-        <v>185</v>
-      </c>
+      <c r="A23" s="33"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="3" t="str">
@@ -1889,9 +1938,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="33" t="s">
-        <v>186</v>
-      </c>
+      <c r="A24" s="33"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="3" t="str">
@@ -1900,9 +1947,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="33" t="s">
-        <v>187</v>
-      </c>
+      <c r="A25" s="33"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="D25" s="3" t="str">
@@ -1911,9 +1956,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="33" t="s">
-        <v>188</v>
-      </c>
+      <c r="A26" s="33"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="D26" s="3" t="str">
@@ -1922,9 +1965,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="33" t="s">
-        <v>189</v>
-      </c>
+      <c r="A27" s="33"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
       <c r="D27" s="3" t="str">
@@ -1933,9 +1974,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="33" t="s">
-        <v>190</v>
-      </c>
+      <c r="A28" s="33"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
       <c r="D28" s="3" t="str">
@@ -1944,9 +1983,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="33" t="s">
-        <v>191</v>
-      </c>
+      <c r="A29" s="33"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="D29" s="3" t="str">
@@ -1955,31 +1992,25 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="33" t="s">
-        <v>192</v>
-      </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
+      <c r="A30" s="33"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
       <c r="D30" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="33" t="s">
-        <v>193</v>
-      </c>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
+      <c r="A31" s="33"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="33"/>
       <c r="D31" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="33" t="s">
-        <v>194</v>
-      </c>
+      <c r="A32" s="33"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
       <c r="D32" s="3" t="str">
@@ -1988,9 +2019,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
-        <v>195</v>
-      </c>
+      <c r="A33" s="33"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
       <c r="D33" s="3" t="str">
@@ -1999,9 +2028,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
-        <v>196</v>
-      </c>
+      <c r="A34" s="8"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
       <c r="D34" s="3" t="str">
@@ -2010,9 +2037,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
-        <v>195</v>
-      </c>
+      <c r="A35" s="7"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
       <c r="D35" s="3" t="str">
@@ -2021,9 +2046,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="7" t="s">
-        <v>197</v>
-      </c>
+      <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
       <c r="D36" s="3" t="str">
@@ -2032,9 +2055,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="7" t="s">
-        <v>198</v>
-      </c>
+      <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
       <c r="D37" s="3" t="str">
@@ -2043,21 +2064,16 @@
       </c>
     </row>
     <row r="38" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="7" t="s">
-        <v>199</v>
-      </c>
+      <c r="A38" s="7"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
       <c r="D38" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E38" s="7"/>
     </row>
     <row r="39" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="7" t="s">
-        <v>200</v>
-      </c>
+      <c r="A39" s="7"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
       <c r="D39" s="3" t="str">
@@ -2067,31 +2083,26 @@
       <c r="E39" s="7"/>
     </row>
     <row r="40" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="7" t="s">
-        <v>201</v>
-      </c>
+      <c r="A40" s="7"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
       <c r="D40" s="3" t="str">
-        <f t="shared" ref="D40:D71" si="2">IF(C40&lt;&gt;"",IF(B40&lt;&gt;"",C40-B40,"-"), "-")</f>
-        <v>-</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="E40" s="7"/>
     </row>
     <row r="41" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="33" t="s">
-        <v>232</v>
-      </c>
+      <c r="A41" s="7"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
       <c r="D41" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="D41:D72" si="2">IF(C41&lt;&gt;"",IF(B41&lt;&gt;"",C41-B41,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="7" t="s">
-        <v>202</v>
-      </c>
+      <c r="A42" s="33"/>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
       <c r="D42" s="3" t="str">
@@ -2100,9 +2111,7 @@
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43" s="7" t="s">
-        <v>203</v>
-      </c>
+      <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
       <c r="D43" s="3" t="str">
@@ -2111,42 +2120,34 @@
       </c>
     </row>
     <row r="44" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="B44" s="8"/>
-      <c r="C44" s="8"/>
+      <c r="A44" s="7"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
       <c r="D44" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="B45" s="33"/>
-      <c r="C45" s="33"/>
+      <c r="A45" s="7"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="8"/>
       <c r="D45" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="B46" s="7"/>
-      <c r="C46" s="7"/>
+      <c r="A46" s="7"/>
+      <c r="B46" s="33"/>
+      <c r="C46" s="33"/>
       <c r="D46" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A47" s="7" t="s">
-        <v>207</v>
-      </c>
+      <c r="A47" s="7"/>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
       <c r="D47" s="3" t="str">
@@ -2155,9 +2156,7 @@
       </c>
     </row>
     <row r="48" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A48" s="7" t="s">
-        <v>208</v>
-      </c>
+      <c r="A48" s="7"/>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
       <c r="D48" s="3" t="str">
@@ -2166,9 +2165,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A49" s="7" t="s">
-        <v>209</v>
-      </c>
+      <c r="A49" s="7"/>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
       <c r="D49" s="3" t="str">
@@ -2177,9 +2174,7 @@
       </c>
     </row>
     <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A50" s="7" t="s">
-        <v>210</v>
-      </c>
+      <c r="A50" s="7"/>
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
       <c r="D50" s="3" t="str">
@@ -2188,9 +2183,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A51" s="7" t="s">
-        <v>211</v>
-      </c>
+      <c r="A51" s="7"/>
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
       <c r="D51" s="3" t="str">
@@ -2199,9 +2192,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A52" s="7" t="s">
-        <v>212</v>
-      </c>
+      <c r="A52" s="7"/>
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
       <c r="D52" s="3" t="str">
@@ -2210,9 +2201,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A53" s="7" t="s">
-        <v>213</v>
-      </c>
+      <c r="A53" s="7"/>
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
       <c r="D53" s="3" t="str">
@@ -2221,9 +2210,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A54" s="7" t="s">
-        <v>214</v>
-      </c>
+      <c r="A54" s="7"/>
       <c r="B54" s="7"/>
       <c r="C54" s="7"/>
       <c r="D54" s="3" t="str">
@@ -2232,9 +2219,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A55" s="7" t="s">
-        <v>215</v>
-      </c>
+      <c r="A55" s="7"/>
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
       <c r="D55" s="3" t="str">
@@ -2243,9 +2228,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A56" s="7" t="s">
-        <v>216</v>
-      </c>
+      <c r="A56" s="7"/>
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
       <c r="D56" s="3" t="str">
@@ -2254,9 +2237,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A57" s="7" t="s">
-        <v>217</v>
-      </c>
+      <c r="A57" s="7"/>
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
       <c r="D57" s="3" t="str">
@@ -2265,9 +2246,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A58" s="7" t="s">
-        <v>218</v>
-      </c>
+      <c r="A58" s="7"/>
       <c r="B58" s="7"/>
       <c r="C58" s="7"/>
       <c r="D58" s="3" t="str">
@@ -2276,9 +2255,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A59" s="7" t="s">
-        <v>219</v>
-      </c>
+      <c r="A59" s="7"/>
       <c r="B59" s="7"/>
       <c r="C59" s="7"/>
       <c r="D59" s="3" t="str">
@@ -2287,9 +2264,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A60" s="7" t="s">
-        <v>220</v>
-      </c>
+      <c r="A60" s="7"/>
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
       <c r="D60" s="3" t="str">
@@ -2298,9 +2273,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A61" s="7" t="s">
-        <v>221</v>
-      </c>
+      <c r="A61" s="7"/>
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
       <c r="D61" s="3" t="str">
@@ -2309,9 +2282,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A62" s="7" t="s">
-        <v>222</v>
-      </c>
+      <c r="A62" s="7"/>
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
       <c r="D62" s="3" t="str">
@@ -2320,9 +2291,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A63" s="7" t="s">
-        <v>223</v>
-      </c>
+      <c r="A63" s="7"/>
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
       <c r="D63" s="3" t="str">
@@ -2331,9 +2300,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A64" s="7" t="s">
-        <v>224</v>
-      </c>
+      <c r="A64" s="7"/>
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
       <c r="D64" s="3" t="str">
@@ -2342,9 +2309,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A65" s="7" t="s">
-        <v>225</v>
-      </c>
+      <c r="A65" s="7"/>
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
       <c r="D65" s="3" t="str">
@@ -2353,9 +2318,7 @@
       </c>
     </row>
     <row r="66" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A66" s="7" t="s">
-        <v>27</v>
-      </c>
+      <c r="A66" s="7"/>
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
       <c r="D66" s="3" t="str">
@@ -2364,9 +2327,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A67" s="7" t="s">
-        <v>226</v>
-      </c>
+      <c r="A67" s="7"/>
       <c r="B67" s="7"/>
       <c r="C67" s="7"/>
       <c r="D67" s="3" t="str">
@@ -2375,9 +2336,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A68" s="34" t="s">
-        <v>234</v>
-      </c>
+      <c r="A68" s="7"/>
       <c r="B68" s="7"/>
       <c r="C68" s="7"/>
       <c r="D68" s="3" t="str">
@@ -2386,9 +2345,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A69" s="34" t="s">
-        <v>233</v>
-      </c>
+      <c r="A69" s="34"/>
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
       <c r="D69" s="3" t="str">
@@ -2397,9 +2354,7 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A70" s="34" t="s">
-        <v>150</v>
-      </c>
+      <c r="A70" s="34"/>
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
       <c r="D70" s="3" t="str">
@@ -2408,9 +2363,7 @@
       </c>
     </row>
     <row r="71" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A71" s="7" t="s">
-        <v>227</v>
-      </c>
+      <c r="A71" s="34"/>
       <c r="B71" s="7"/>
       <c r="C71" s="7"/>
       <c r="D71" s="3" t="str">
@@ -2419,64 +2372,52 @@
       </c>
     </row>
     <row r="72" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A72" s="7" t="s">
-        <v>228</v>
-      </c>
+      <c r="A72" s="7"/>
       <c r="B72" s="7"/>
       <c r="C72" s="7"/>
       <c r="D72" s="3" t="str">
-        <f t="shared" ref="D72:D78" si="3">IF(C72&lt;&gt;"",IF(B72&lt;&gt;"",C72-B72,"-"), "-")</f>
+        <f t="shared" si="2"/>
         <v>-</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A73" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="B73" s="9"/>
-      <c r="C73" s="9"/>
+      <c r="A73" s="7"/>
+      <c r="B73" s="7"/>
+      <c r="C73" s="7"/>
       <c r="D73" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="D73:D79" si="3">IF(C73&lt;&gt;"",IF(B73&lt;&gt;"",C73-B73,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A74" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="B74" s="7"/>
-      <c r="C74" s="7"/>
+      <c r="A74" s="7"/>
+      <c r="B74" s="9"/>
+      <c r="C74" s="9"/>
       <c r="D74" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A75" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="B75" s="9"/>
-      <c r="C75" s="9"/>
+      <c r="A75" s="7"/>
+      <c r="B75" s="7"/>
+      <c r="C75" s="7"/>
       <c r="D75" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A76" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="B76" s="7"/>
-      <c r="C76" s="7"/>
+      <c r="A76" s="7"/>
+      <c r="B76" s="9"/>
+      <c r="C76" s="9"/>
       <c r="D76" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A77" s="7" t="s">
-        <v>124</v>
-      </c>
+      <c r="A77" s="7"/>
       <c r="B77" s="7"/>
       <c r="C77" s="7"/>
       <c r="D77" s="3" t="str">
@@ -2485,9 +2426,7 @@
       </c>
     </row>
     <row r="78" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A78" s="5" t="s">
-        <v>10</v>
-      </c>
+      <c r="A78" s="7"/>
       <c r="B78" s="7"/>
       <c r="C78" s="7"/>
       <c r="D78" s="3" t="str">
@@ -2496,31 +2435,25 @@
       </c>
     </row>
     <row r="79" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A79" s="5" t="s">
-        <v>31</v>
-      </c>
+      <c r="A79" s="5"/>
       <c r="B79" s="7"/>
       <c r="C79" s="7"/>
       <c r="D79" s="3" t="str">
-        <f t="shared" ref="D79:D147" si="4">IF(C79&lt;&gt;"",IF(B79&lt;&gt;"",C79-B79,"-"), "-")</f>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A80" s="5" t="s">
-        <v>11</v>
-      </c>
+      <c r="A80" s="5"/>
       <c r="B80" s="7"/>
       <c r="C80" s="7"/>
       <c r="D80" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="D80:D148" si="4">IF(C80&lt;&gt;"",IF(B80&lt;&gt;"",C80-B80,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A81" s="5" t="s">
-        <v>30</v>
-      </c>
+      <c r="A81" s="5"/>
       <c r="B81" s="7"/>
       <c r="C81" s="7"/>
       <c r="D81" s="3" t="str">
@@ -2529,9 +2462,7 @@
       </c>
     </row>
     <row r="82" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A82" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="A82" s="5"/>
       <c r="B82" s="7"/>
       <c r="C82" s="7"/>
       <c r="D82" s="3" t="str">
@@ -2540,9 +2471,7 @@
       </c>
     </row>
     <row r="83" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A83" s="5" t="s">
-        <v>32</v>
-      </c>
+      <c r="A83" s="5"/>
       <c r="B83" s="7"/>
       <c r="C83" s="7"/>
       <c r="D83" s="3" t="str">
@@ -2551,9 +2480,7 @@
       </c>
     </row>
     <row r="84" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A84" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="A84" s="5"/>
       <c r="B84" s="7"/>
       <c r="C84" s="7"/>
       <c r="D84" s="3" t="str">
@@ -2562,9 +2489,7 @@
       </c>
     </row>
     <row r="85" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A85" s="7" t="s">
-        <v>47</v>
-      </c>
+      <c r="A85" s="5"/>
       <c r="B85" s="7"/>
       <c r="C85" s="7"/>
       <c r="D85" s="3" t="str">
@@ -2573,9 +2498,7 @@
       </c>
     </row>
     <row r="86" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A86" s="7" t="s">
-        <v>48</v>
-      </c>
+      <c r="A86" s="7"/>
       <c r="B86" s="7"/>
       <c r="C86" s="7"/>
       <c r="D86" s="3" t="str">
@@ -2584,9 +2507,7 @@
       </c>
     </row>
     <row r="87" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A87" s="34" t="s">
-        <v>235</v>
-      </c>
+      <c r="A87" s="7"/>
       <c r="B87" s="7"/>
       <c r="C87" s="7"/>
       <c r="D87" s="3" t="str">
@@ -2595,9 +2516,7 @@
       </c>
     </row>
     <row r="88" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A88" s="7" t="s">
-        <v>33</v>
-      </c>
+      <c r="A88" s="34"/>
       <c r="B88" s="7"/>
       <c r="C88" s="7"/>
       <c r="D88" s="3" t="str">
@@ -2606,9 +2525,7 @@
       </c>
     </row>
     <row r="89" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A89" s="5" t="s">
-        <v>14</v>
-      </c>
+      <c r="A89" s="7"/>
       <c r="B89" s="7"/>
       <c r="C89" s="7"/>
       <c r="D89" s="3" t="str">
@@ -2617,9 +2534,7 @@
       </c>
     </row>
     <row r="90" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A90" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="A90" s="5"/>
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
       <c r="D90" s="3" t="str">
@@ -2628,9 +2543,7 @@
       </c>
     </row>
     <row r="91" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A91" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="A91" s="5"/>
       <c r="B91" s="7"/>
       <c r="C91" s="7"/>
       <c r="D91" s="3" t="str">
@@ -2639,9 +2552,7 @@
       </c>
     </row>
     <row r="92" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A92" s="5" t="s">
-        <v>35</v>
-      </c>
+      <c r="A92" s="5"/>
       <c r="B92" s="7"/>
       <c r="C92" s="7"/>
       <c r="D92" s="3" t="str">
@@ -2650,9 +2561,7 @@
       </c>
     </row>
     <row r="93" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A93" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="A93" s="5"/>
       <c r="B93" s="7"/>
       <c r="C93" s="7"/>
       <c r="D93" s="3" t="str">
@@ -2661,9 +2570,7 @@
       </c>
     </row>
     <row r="94" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A94" s="5" t="s">
-        <v>36</v>
-      </c>
+      <c r="A94" s="5"/>
       <c r="B94" s="7"/>
       <c r="C94" s="7"/>
       <c r="D94" s="3" t="str">
@@ -2672,9 +2579,7 @@
       </c>
     </row>
     <row r="95" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A95" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="A95" s="5"/>
       <c r="B95" s="7"/>
       <c r="C95" s="7"/>
       <c r="D95" s="3" t="str">
@@ -2683,9 +2588,7 @@
       </c>
     </row>
     <row r="96" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A96" s="5" t="s">
-        <v>37</v>
-      </c>
+      <c r="A96" s="5"/>
       <c r="B96" s="7"/>
       <c r="C96" s="7"/>
       <c r="D96" s="3" t="str">
@@ -2694,9 +2597,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A97" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="A97" s="5"/>
       <c r="B97" s="7"/>
       <c r="C97" s="7"/>
       <c r="D97" s="3" t="str">
@@ -2705,9 +2606,7 @@
       </c>
     </row>
     <row r="98" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A98" s="5" t="s">
-        <v>38</v>
-      </c>
+      <c r="A98" s="5"/>
       <c r="B98" s="7"/>
       <c r="C98" s="7"/>
       <c r="D98" s="3" t="str">
@@ -2716,9 +2615,7 @@
       </c>
     </row>
     <row r="99" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A99" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="A99" s="5"/>
       <c r="B99" s="7"/>
       <c r="C99" s="7"/>
       <c r="D99" s="3" t="str">
@@ -2727,9 +2624,7 @@
       </c>
     </row>
     <row r="100" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A100" s="5" t="s">
-        <v>39</v>
-      </c>
+      <c r="A100" s="5"/>
       <c r="B100" s="7"/>
       <c r="C100" s="7"/>
       <c r="D100" s="3" t="str">
@@ -2738,9 +2633,7 @@
       </c>
     </row>
     <row r="101" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A101" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="A101" s="5"/>
       <c r="B101" s="7"/>
       <c r="C101" s="7"/>
       <c r="D101" s="3" t="str">
@@ -2749,9 +2642,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A102" s="5" t="s">
-        <v>40</v>
-      </c>
+      <c r="A102" s="5"/>
       <c r="B102" s="7"/>
       <c r="C102" s="7"/>
       <c r="D102" s="3" t="str">
@@ -2760,9 +2651,7 @@
       </c>
     </row>
     <row r="103" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A103" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="A103" s="5"/>
       <c r="B103" s="7"/>
       <c r="C103" s="7"/>
       <c r="D103" s="3" t="str">
@@ -2771,9 +2660,7 @@
       </c>
     </row>
     <row r="104" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A104" s="5" t="s">
-        <v>41</v>
-      </c>
+      <c r="A104" s="5"/>
       <c r="B104" s="7"/>
       <c r="C104" s="7"/>
       <c r="D104" s="3" t="str">
@@ -2782,9 +2669,7 @@
       </c>
     </row>
     <row r="105" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A105" s="5" t="s">
-        <v>22</v>
-      </c>
+      <c r="A105" s="5"/>
       <c r="B105" s="7"/>
       <c r="C105" s="7"/>
       <c r="D105" s="3" t="str">
@@ -2793,31 +2678,25 @@
       </c>
     </row>
     <row r="106" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A106" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B106" s="10"/>
-      <c r="C106" s="10"/>
+      <c r="A106" s="5"/>
+      <c r="B106" s="7"/>
+      <c r="C106" s="7"/>
       <c r="D106" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A107" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B107" s="7"/>
-      <c r="C107" s="7"/>
+      <c r="A107" s="5"/>
+      <c r="B107" s="10"/>
+      <c r="C107" s="10"/>
       <c r="D107" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A108" s="35" t="s">
-        <v>127</v>
-      </c>
+      <c r="A108" s="5"/>
       <c r="B108" s="7"/>
       <c r="C108" s="7"/>
       <c r="D108" s="3" t="str">
@@ -2826,9 +2705,7 @@
       </c>
     </row>
     <row r="109" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A109" s="5" t="s">
-        <v>43</v>
-      </c>
+      <c r="A109" s="35"/>
       <c r="B109" s="7"/>
       <c r="C109" s="7"/>
       <c r="D109" s="3" t="str">
@@ -2837,9 +2714,7 @@
       </c>
     </row>
     <row r="110" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A110" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="A110" s="5"/>
       <c r="B110" s="7"/>
       <c r="C110" s="7"/>
       <c r="D110" s="3" t="str">
@@ -2848,9 +2723,7 @@
       </c>
     </row>
     <row r="111" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A111" s="5" t="s">
-        <v>44</v>
-      </c>
+      <c r="A111" s="5"/>
       <c r="B111" s="7"/>
       <c r="C111" s="7"/>
       <c r="D111" s="3" t="str">
@@ -2859,9 +2732,7 @@
       </c>
     </row>
     <row r="112" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A112" s="5" t="s">
-        <v>25</v>
-      </c>
+      <c r="A112" s="5"/>
       <c r="B112" s="7"/>
       <c r="C112" s="7"/>
       <c r="D112" s="3" t="str">
@@ -2873,7 +2744,10 @@
       <c r="A113" s="5"/>
       <c r="B113" s="7"/>
       <c r="C113" s="7"/>
-      <c r="D113" s="3"/>
+      <c r="D113" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="114" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A114" s="5"/>
@@ -2888,20 +2762,19 @@
       <c r="D115" s="3"/>
     </row>
     <row r="116" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A116" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="A116" s="5"/>
       <c r="B116" s="7"/>
       <c r="C116" s="7"/>
-      <c r="D116" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v>-</v>
-      </c>
+      <c r="D116" s="3"/>
     </row>
     <row r="117" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A117" s="7"/>
+      <c r="A117" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="B117" s="7"/>
-      <c r="C117" s="7"/>
+      <c r="C117" s="7">
+        <v>63782</v>
+      </c>
       <c r="D117" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
@@ -3182,7 +3055,7 @@
       <c r="B148" s="7"/>
       <c r="C148" s="7"/>
       <c r="D148" s="3" t="str">
-        <f t="shared" ref="D148:D152" si="5">IF(C148&lt;&gt;"",IF(B148&lt;&gt;"",C148-B148,"-"), "-")</f>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
     </row>
@@ -3191,7 +3064,7 @@
       <c r="B149" s="7"/>
       <c r="C149" s="7"/>
       <c r="D149" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="D149:D153" si="5">IF(C149&lt;&gt;"",IF(B149&lt;&gt;"",C149-B149,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
@@ -3227,7 +3100,7 @@
       <c r="B153" s="7"/>
       <c r="C153" s="7"/>
       <c r="D153" s="3" t="str">
-        <f t="shared" ref="D153:D154" si="6">IF(C153&lt;&gt;"",IF(B153&lt;&gt;"",B153-C153,"-"), "-")</f>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
     </row>
@@ -3236,7 +3109,7 @@
       <c r="B154" s="7"/>
       <c r="C154" s="7"/>
       <c r="D154" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="D154:D155" si="6">IF(C154&lt;&gt;"",IF(B154&lt;&gt;"",B154-C154,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
@@ -3244,6 +3117,10 @@
       <c r="A155" s="7"/>
       <c r="B155" s="7"/>
       <c r="C155" s="7"/>
+      <c r="D155" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="156" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A156" s="7"/>
@@ -3251,6 +3128,7 @@
       <c r="C156" s="7"/>
     </row>
     <row r="157" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A157" s="7"/>
       <c r="B157" s="7"/>
       <c r="C157" s="7"/>
     </row>
@@ -3797,6 +3675,10 @@
     <row r="293" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B293" s="7"/>
       <c r="C293" s="7"/>
+    </row>
+    <row r="294" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B294" s="7"/>
+      <c r="C294" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
lode runner up to start of level 10, 2990 frames ahead
</commit_message>
<xml_diff>
--- a/LodeRunner/compare.xlsx
+++ b/LodeRunner/compare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\LodeRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38760631-5265-4ECA-9981-51912F764CE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591030D0-5156-463C-9107-95F3AD4FF983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="50865" yWindow="3795" windowWidth="7170" windowHeight="12990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="276">
   <si>
     <t>Place</t>
   </si>
@@ -794,6 +794,75 @@
   </si>
   <si>
     <t>04 1st move</t>
+  </si>
+  <si>
+    <t>04 end</t>
+  </si>
+  <si>
+    <t>05 ladder grab</t>
+  </si>
+  <si>
+    <t>05 end</t>
+  </si>
+  <si>
+    <t>06 1st dig</t>
+  </si>
+  <si>
+    <t>06 end</t>
+  </si>
+  <si>
+    <t>07 1st move</t>
+  </si>
+  <si>
+    <t>07 end</t>
+  </si>
+  <si>
+    <t>4th dig</t>
+  </si>
+  <si>
+    <t>2nd dig</t>
+  </si>
+  <si>
+    <t>5th dig</t>
+  </si>
+  <si>
+    <t>need to delay for enemy at top to go right, saving a longer delay on the ladder</t>
+  </si>
+  <si>
+    <t>08 ladder grab</t>
+  </si>
+  <si>
+    <t>ladder grab</t>
+  </si>
+  <si>
+    <t>3rd dig</t>
+  </si>
+  <si>
+    <t>08 end</t>
+  </si>
+  <si>
+    <t>09 ladder grab</t>
+  </si>
+  <si>
+    <t>2nd ladder grab</t>
+  </si>
+  <si>
+    <t>3rd ladder grab</t>
+  </si>
+  <si>
+    <t>last dig</t>
+  </si>
+  <si>
+    <t>1st 3rd cycle dig</t>
+  </si>
+  <si>
+    <t>2nd to last</t>
+  </si>
+  <si>
+    <t>09 end</t>
+  </si>
+  <si>
+    <t>10 grab ladder</t>
   </si>
 </sst>
 </file>
@@ -1601,11 +1670,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB48F502-AA0A-4BF9-ABA2-AA87E3F2B5E4}">
-  <dimension ref="A1:E294"/>
+  <dimension ref="A1:E298"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1641,7 +1710,7 @@
         <v>426</v>
       </c>
       <c r="D2" s="3">
-        <f t="shared" ref="D2:D40" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
+        <f t="shared" ref="D2:D44" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
         <v>1</v>
       </c>
     </row>
@@ -1856,7 +1925,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="45" t="s">
         <v>250</v>
       </c>
@@ -1871,7 +1940,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="45" t="s">
         <v>251</v>
       </c>
@@ -1886,7 +1955,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="45" t="s">
         <v>252</v>
       </c>
@@ -1901,246 +1970,399 @@
         <v>1182</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="33"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="33"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="33"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="33"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="33"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="33"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="33"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="33"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="33"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="33"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="33"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="33"/>
-      <c r="B31" s="33"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="33"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="45" t="s">
+        <v>127</v>
+      </c>
+      <c r="B20" s="7">
+        <v>2812</v>
+      </c>
+      <c r="C20" s="7">
+        <v>3994</v>
+      </c>
+      <c r="D20" s="3">
+        <f t="shared" si="0"/>
+        <v>1182</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="45" t="s">
+        <v>253</v>
+      </c>
+      <c r="B21" s="7">
+        <v>3195</v>
+      </c>
+      <c r="C21" s="7">
+        <v>4382</v>
+      </c>
+      <c r="D21" s="3">
+        <f t="shared" si="0"/>
+        <v>1187</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="45" t="s">
+        <v>254</v>
+      </c>
+      <c r="B22" s="7">
+        <v>3566</v>
+      </c>
+      <c r="C22" s="7">
+        <v>5071</v>
+      </c>
+      <c r="D22" s="3">
+        <f t="shared" si="0"/>
+        <v>1505</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="45" t="s">
+        <v>255</v>
+      </c>
+      <c r="B23" s="7">
+        <v>3829</v>
+      </c>
+      <c r="C23" s="7">
+        <v>5328</v>
+      </c>
+      <c r="D23" s="3">
+        <f t="shared" si="0"/>
+        <v>1499</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="45" t="s">
+        <v>256</v>
+      </c>
+      <c r="B24" s="7">
+        <v>4183</v>
+      </c>
+      <c r="C24" s="7">
+        <v>5985</v>
+      </c>
+      <c r="D24" s="3">
+        <f t="shared" si="0"/>
+        <v>1802</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="45" t="s">
+        <v>257</v>
+      </c>
+      <c r="B25" s="7">
+        <v>5182</v>
+      </c>
+      <c r="C25" s="7">
+        <v>6992</v>
+      </c>
+      <c r="D25" s="3">
+        <f t="shared" si="0"/>
+        <v>1810</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="45" t="s">
+        <v>258</v>
+      </c>
+      <c r="B26" s="7">
+        <v>5541</v>
+      </c>
+      <c r="C26" s="7">
+        <v>7647</v>
+      </c>
+      <c r="D26" s="3">
+        <f t="shared" si="0"/>
+        <v>2106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="45" t="s">
+        <v>127</v>
+      </c>
+      <c r="B27" s="7">
+        <v>5561</v>
+      </c>
+      <c r="C27" s="7">
+        <v>7667</v>
+      </c>
+      <c r="D27" s="3">
+        <f t="shared" si="0"/>
+        <v>2106</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="45" t="s">
+        <v>261</v>
+      </c>
+      <c r="B28" s="7">
+        <v>5663</v>
+      </c>
+      <c r="C28" s="7">
+        <v>7771</v>
+      </c>
+      <c r="D28" s="3">
+        <f t="shared" si="0"/>
+        <v>2108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="45" t="s">
+        <v>260</v>
+      </c>
+      <c r="B29" s="7">
+        <v>5721</v>
+      </c>
+      <c r="C29" s="7">
+        <v>7829</v>
+      </c>
+      <c r="D29" s="3">
+        <f t="shared" si="0"/>
+        <v>2108</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="45" t="s">
+        <v>262</v>
+      </c>
+      <c r="B30" s="7">
+        <v>5757</v>
+      </c>
+      <c r="C30" s="7">
+        <v>7863</v>
+      </c>
+      <c r="D30" s="3">
+        <f t="shared" si="0"/>
+        <v>2106</v>
+      </c>
+      <c r="E30" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="45" t="s">
+        <v>259</v>
+      </c>
+      <c r="B31" s="7">
+        <v>6002</v>
+      </c>
+      <c r="C31" s="7">
+        <v>8106</v>
+      </c>
+      <c r="D31" s="3">
+        <f t="shared" si="0"/>
+        <v>2104</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="45" t="s">
+        <v>264</v>
+      </c>
+      <c r="B32" s="7">
+        <v>6361</v>
+      </c>
+      <c r="C32" s="7">
+        <v>8766</v>
+      </c>
+      <c r="D32" s="3">
+        <f t="shared" si="0"/>
+        <v>2405</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="33"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A33" s="45" t="s">
+        <v>261</v>
+      </c>
+      <c r="B33" s="7">
+        <v>6434</v>
+      </c>
+      <c r="C33" s="7">
+        <v>8839</v>
+      </c>
+      <c r="D33" s="3">
+        <f t="shared" si="0"/>
+        <v>2405</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="8"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A34" s="45" t="s">
+        <v>265</v>
+      </c>
+      <c r="B34" s="7">
+        <v>6552</v>
+      </c>
+      <c r="C34" s="7">
+        <v>8951</v>
+      </c>
+      <c r="D34" s="3">
+        <f t="shared" si="0"/>
+        <v>2399</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A35" s="45" t="s">
+        <v>266</v>
+      </c>
+      <c r="B35" s="33">
+        <v>6579</v>
+      </c>
+      <c r="C35" s="33">
+        <v>8978</v>
+      </c>
+      <c r="D35" s="3">
+        <f t="shared" si="0"/>
+        <v>2399</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A36" s="45" t="s">
+        <v>267</v>
+      </c>
+      <c r="B36" s="7">
+        <v>6759</v>
+      </c>
+      <c r="C36" s="7">
+        <v>9159</v>
+      </c>
+      <c r="D36" s="3">
+        <f t="shared" si="0"/>
+        <v>2400</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="7"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A37" s="45" t="s">
+        <v>268</v>
+      </c>
+      <c r="B37" s="7">
+        <v>7126</v>
+      </c>
+      <c r="C37" s="7">
+        <v>9831</v>
+      </c>
+      <c r="D37" s="3">
+        <f t="shared" si="0"/>
+        <v>2705</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="7"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A38" s="45" t="s">
+        <v>269</v>
+      </c>
+      <c r="B38" s="7">
+        <v>7531</v>
+      </c>
+      <c r="C38" s="45">
+        <v>10236</v>
+      </c>
+      <c r="D38" s="3">
+        <f t="shared" si="0"/>
+        <v>2705</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="E39" s="7"/>
+      <c r="A39" s="45" t="s">
+        <v>270</v>
+      </c>
+      <c r="B39" s="7">
+        <v>7843</v>
+      </c>
+      <c r="C39" s="7">
+        <v>10550</v>
+      </c>
+      <c r="D39" s="3">
+        <f t="shared" si="0"/>
+        <v>2707</v>
+      </c>
     </row>
     <row r="40" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="7"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="E40" s="7"/>
+      <c r="A40" s="45" t="s">
+        <v>272</v>
+      </c>
+      <c r="B40" s="7">
+        <v>7921</v>
+      </c>
+      <c r="C40" s="7">
+        <v>10626</v>
+      </c>
+      <c r="D40" s="3">
+        <f t="shared" si="0"/>
+        <v>2705</v>
+      </c>
     </row>
     <row r="41" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="7"/>
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="3" t="str">
-        <f t="shared" ref="D41:D72" si="2">IF(C41&lt;&gt;"",IF(B41&lt;&gt;"",C41-B41,"-"), "-")</f>
-        <v>-</v>
+      <c r="A41" s="45" t="s">
+        <v>273</v>
+      </c>
+      <c r="B41" s="7">
+        <v>8065</v>
+      </c>
+      <c r="C41" s="7">
+        <v>10769</v>
+      </c>
+      <c r="D41" s="3">
+        <f t="shared" si="0"/>
+        <v>2704</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="33"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
+      <c r="A42" s="45" t="s">
+        <v>271</v>
+      </c>
+      <c r="B42" s="7">
+        <v>8097</v>
+      </c>
+      <c r="C42" s="7">
+        <v>10801</v>
+      </c>
+      <c r="D42" s="3">
+        <f t="shared" si="0"/>
+        <v>2704</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43" s="7"/>
-      <c r="B43" s="7"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
+      <c r="A43" s="45" t="s">
+        <v>274</v>
+      </c>
+      <c r="B43" s="7">
+        <v>8191</v>
+      </c>
+      <c r="C43" s="7">
+        <v>10896</v>
+      </c>
+      <c r="D43" s="3">
+        <f t="shared" si="0"/>
+        <v>2705</v>
+      </c>
+      <c r="E43" s="7"/>
     </row>
     <row r="44" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="7"/>
-      <c r="B44" s="7"/>
-      <c r="C44" s="7"/>
-      <c r="D44" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
+      <c r="A44" s="45" t="s">
+        <v>275</v>
+      </c>
+      <c r="B44" s="7">
+        <v>8555</v>
+      </c>
+      <c r="C44" s="7">
+        <v>11545</v>
+      </c>
+      <c r="D44" s="3">
+        <f t="shared" si="0"/>
+        <v>2990</v>
+      </c>
+      <c r="E44" s="7"/>
     </row>
     <row r="45" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
       <c r="D45" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="D45:D76" si="2">IF(C45&lt;&gt;"",IF(B45&lt;&gt;"",C45-B45,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="7"/>
-      <c r="B46" s="33"/>
-      <c r="C46" s="33"/>
+      <c r="A46" s="33"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="7"/>
       <c r="D46" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2166,8 +2388,8 @@
     </row>
     <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
-      <c r="B49" s="7"/>
-      <c r="C49" s="7"/>
+      <c r="B49" s="8"/>
+      <c r="C49" s="8"/>
       <c r="D49" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2175,8 +2397,8 @@
     </row>
     <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="7"/>
-      <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
+      <c r="B50" s="33"/>
+      <c r="C50" s="33"/>
       <c r="D50" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2345,7 +2567,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A69" s="34"/>
+      <c r="A69" s="7"/>
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
       <c r="D69" s="3" t="str">
@@ -2354,7 +2576,7 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A70" s="34"/>
+      <c r="A70" s="7"/>
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
       <c r="D70" s="3" t="str">
@@ -2363,7 +2585,7 @@
       </c>
     </row>
     <row r="71" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A71" s="34"/>
+      <c r="A71" s="7"/>
       <c r="B71" s="7"/>
       <c r="C71" s="7"/>
       <c r="D71" s="3" t="str">
@@ -2381,38 +2603,38 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A73" s="7"/>
+      <c r="A73" s="34"/>
       <c r="B73" s="7"/>
       <c r="C73" s="7"/>
       <c r="D73" s="3" t="str">
-        <f t="shared" ref="D73:D79" si="3">IF(C73&lt;&gt;"",IF(B73&lt;&gt;"",C73-B73,"-"), "-")</f>
+        <f t="shared" si="2"/>
         <v>-</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A74" s="7"/>
-      <c r="B74" s="9"/>
-      <c r="C74" s="9"/>
+      <c r="A74" s="34"/>
+      <c r="B74" s="7"/>
+      <c r="C74" s="7"/>
       <c r="D74" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A75" s="7"/>
+      <c r="A75" s="34"/>
       <c r="B75" s="7"/>
       <c r="C75" s="7"/>
       <c r="D75" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="7"/>
-      <c r="B76" s="9"/>
-      <c r="C76" s="9"/>
+      <c r="B76" s="7"/>
+      <c r="C76" s="7"/>
       <c r="D76" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-</v>
       </c>
     </row>
@@ -2421,21 +2643,21 @@
       <c r="B77" s="7"/>
       <c r="C77" s="7"/>
       <c r="D77" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="D77:D83" si="3">IF(C77&lt;&gt;"",IF(B77&lt;&gt;"",C77-B77,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="7"/>
-      <c r="B78" s="7"/>
-      <c r="C78" s="7"/>
+      <c r="B78" s="9"/>
+      <c r="C78" s="9"/>
       <c r="D78" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A79" s="5"/>
+      <c r="A79" s="7"/>
       <c r="B79" s="7"/>
       <c r="C79" s="7"/>
       <c r="D79" s="3" t="str">
@@ -2444,29 +2666,29 @@
       </c>
     </row>
     <row r="80" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A80" s="5"/>
-      <c r="B80" s="7"/>
-      <c r="C80" s="7"/>
+      <c r="A80" s="7"/>
+      <c r="B80" s="9"/>
+      <c r="C80" s="9"/>
       <c r="D80" s="3" t="str">
-        <f t="shared" ref="D80:D148" si="4">IF(C80&lt;&gt;"",IF(B80&lt;&gt;"",C80-B80,"-"), "-")</f>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A81" s="5"/>
+      <c r="A81" s="7"/>
       <c r="B81" s="7"/>
       <c r="C81" s="7"/>
       <c r="D81" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A82" s="5"/>
+      <c r="A82" s="7"/>
       <c r="B82" s="7"/>
       <c r="C82" s="7"/>
       <c r="D82" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
     </row>
@@ -2475,7 +2697,7 @@
       <c r="B83" s="7"/>
       <c r="C83" s="7"/>
       <c r="D83" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
     </row>
@@ -2484,7 +2706,7 @@
       <c r="B84" s="7"/>
       <c r="C84" s="7"/>
       <c r="D84" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="D84:D152" si="4">IF(C84&lt;&gt;"",IF(B84&lt;&gt;"",C84-B84,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
@@ -2498,7 +2720,7 @@
       </c>
     </row>
     <row r="86" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A86" s="7"/>
+      <c r="A86" s="5"/>
       <c r="B86" s="7"/>
       <c r="C86" s="7"/>
       <c r="D86" s="3" t="str">
@@ -2507,7 +2729,7 @@
       </c>
     </row>
     <row r="87" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A87" s="7"/>
+      <c r="A87" s="5"/>
       <c r="B87" s="7"/>
       <c r="C87" s="7"/>
       <c r="D87" s="3" t="str">
@@ -2516,7 +2738,7 @@
       </c>
     </row>
     <row r="88" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A88" s="34"/>
+      <c r="A88" s="5"/>
       <c r="B88" s="7"/>
       <c r="C88" s="7"/>
       <c r="D88" s="3" t="str">
@@ -2525,7 +2747,7 @@
       </c>
     </row>
     <row r="89" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A89" s="7"/>
+      <c r="A89" s="5"/>
       <c r="B89" s="7"/>
       <c r="C89" s="7"/>
       <c r="D89" s="3" t="str">
@@ -2534,7 +2756,7 @@
       </c>
     </row>
     <row r="90" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A90" s="5"/>
+      <c r="A90" s="7"/>
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
       <c r="D90" s="3" t="str">
@@ -2543,7 +2765,7 @@
       </c>
     </row>
     <row r="91" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A91" s="5"/>
+      <c r="A91" s="7"/>
       <c r="B91" s="7"/>
       <c r="C91" s="7"/>
       <c r="D91" s="3" t="str">
@@ -2552,7 +2774,7 @@
       </c>
     </row>
     <row r="92" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A92" s="5"/>
+      <c r="A92" s="34"/>
       <c r="B92" s="7"/>
       <c r="C92" s="7"/>
       <c r="D92" s="3" t="str">
@@ -2561,7 +2783,7 @@
       </c>
     </row>
     <row r="93" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A93" s="5"/>
+      <c r="A93" s="7"/>
       <c r="B93" s="7"/>
       <c r="C93" s="7"/>
       <c r="D93" s="3" t="str">
@@ -2688,8 +2910,8 @@
     </row>
     <row r="107" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A107" s="5"/>
-      <c r="B107" s="10"/>
-      <c r="C107" s="10"/>
+      <c r="B107" s="7"/>
+      <c r="C107" s="7"/>
       <c r="D107" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
@@ -2705,7 +2927,7 @@
       </c>
     </row>
     <row r="109" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A109" s="35"/>
+      <c r="A109" s="5"/>
       <c r="B109" s="7"/>
       <c r="C109" s="7"/>
       <c r="D109" s="3" t="str">
@@ -2724,8 +2946,8 @@
     </row>
     <row r="111" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A111" s="5"/>
-      <c r="B111" s="7"/>
-      <c r="C111" s="7"/>
+      <c r="B111" s="10"/>
+      <c r="C111" s="10"/>
       <c r="D111" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
@@ -2741,7 +2963,7 @@
       </c>
     </row>
     <row r="113" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A113" s="5"/>
+      <c r="A113" s="35"/>
       <c r="B113" s="7"/>
       <c r="C113" s="7"/>
       <c r="D113" s="3" t="str">
@@ -2753,64 +2975,64 @@
       <c r="A114" s="5"/>
       <c r="B114" s="7"/>
       <c r="C114" s="7"/>
-      <c r="D114" s="3"/>
+      <c r="D114" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="115" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A115" s="5"/>
       <c r="B115" s="7"/>
       <c r="C115" s="7"/>
-      <c r="D115" s="3"/>
+      <c r="D115" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="116" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A116" s="5"/>
       <c r="B116" s="7"/>
       <c r="C116" s="7"/>
-      <c r="D116" s="3"/>
+      <c r="D116" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="117" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A117" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="A117" s="5"/>
       <c r="B117" s="7"/>
-      <c r="C117" s="7">
-        <v>63782</v>
-      </c>
+      <c r="C117" s="7"/>
       <c r="D117" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A118" s="7"/>
+      <c r="A118" s="5"/>
       <c r="B118" s="7"/>
       <c r="C118" s="7"/>
-      <c r="D118" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v>-</v>
-      </c>
+      <c r="D118" s="3"/>
     </row>
     <row r="119" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A119" s="7"/>
+      <c r="A119" s="5"/>
       <c r="B119" s="7"/>
       <c r="C119" s="7"/>
-      <c r="D119" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v>-</v>
-      </c>
+      <c r="D119" s="3"/>
     </row>
     <row r="120" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A120" s="7"/>
+      <c r="A120" s="5"/>
       <c r="B120" s="7"/>
       <c r="C120" s="7"/>
-      <c r="D120" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v>-</v>
-      </c>
+      <c r="D120" s="3"/>
     </row>
     <row r="121" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A121" s="7"/>
+      <c r="A121" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="B121" s="7"/>
-      <c r="C121" s="7"/>
+      <c r="C121" s="7">
+        <v>63782</v>
+      </c>
       <c r="D121" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
@@ -3064,7 +3286,7 @@
       <c r="B149" s="7"/>
       <c r="C149" s="7"/>
       <c r="D149" s="3" t="str">
-        <f t="shared" ref="D149:D153" si="5">IF(C149&lt;&gt;"",IF(B149&lt;&gt;"",C149-B149,"-"), "-")</f>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
     </row>
@@ -3073,7 +3295,7 @@
       <c r="B150" s="7"/>
       <c r="C150" s="7"/>
       <c r="D150" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
     </row>
@@ -3082,7 +3304,7 @@
       <c r="B151" s="7"/>
       <c r="C151" s="7"/>
       <c r="D151" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
     </row>
@@ -3091,7 +3313,7 @@
       <c r="B152" s="7"/>
       <c r="C152" s="7"/>
       <c r="D152" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
     </row>
@@ -3100,7 +3322,7 @@
       <c r="B153" s="7"/>
       <c r="C153" s="7"/>
       <c r="D153" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="D153:D157" si="5">IF(C153&lt;&gt;"",IF(B153&lt;&gt;"",C153-B153,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
@@ -3109,7 +3331,7 @@
       <c r="B154" s="7"/>
       <c r="C154" s="7"/>
       <c r="D154" s="3" t="str">
-        <f t="shared" ref="D154:D155" si="6">IF(C154&lt;&gt;"",IF(B154&lt;&gt;"",B154-C154,"-"), "-")</f>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
     </row>
@@ -3118,7 +3340,7 @@
       <c r="B155" s="7"/>
       <c r="C155" s="7"/>
       <c r="D155" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
     </row>
@@ -3126,85 +3348,105 @@
       <c r="A156" s="7"/>
       <c r="B156" s="7"/>
       <c r="C156" s="7"/>
+      <c r="D156" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="157" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A157" s="7"/>
       <c r="B157" s="7"/>
       <c r="C157" s="7"/>
+      <c r="D157" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="158" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A158" s="7"/>
       <c r="B158" s="7"/>
       <c r="C158" s="7"/>
+      <c r="D158" s="3" t="str">
+        <f t="shared" ref="D158:D159" si="6">IF(C158&lt;&gt;"",IF(B158&lt;&gt;"",B158-C158,"-"), "-")</f>
+        <v>-</v>
+      </c>
     </row>
     <row r="159" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A159" s="7"/>
       <c r="B159" s="7"/>
       <c r="C159" s="7"/>
+      <c r="D159" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="160" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A160" s="7"/>
       <c r="B160" s="7"/>
       <c r="C160" s="7"/>
     </row>
-    <row r="161" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A161" s="7"/>
       <c r="B161" s="7"/>
       <c r="C161" s="7"/>
     </row>
-    <row r="162" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B162" s="7"/>
       <c r="C162" s="7"/>
     </row>
-    <row r="163" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B163" s="7"/>
       <c r="C163" s="7"/>
     </row>
-    <row r="164" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B164" s="7"/>
       <c r="C164" s="7"/>
     </row>
-    <row r="165" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B165" s="7"/>
       <c r="C165" s="7"/>
     </row>
-    <row r="166" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B166" s="7"/>
       <c r="C166" s="7"/>
     </row>
-    <row r="167" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B167" s="7"/>
       <c r="C167" s="7"/>
     </row>
-    <row r="168" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B168" s="7"/>
       <c r="C168" s="7"/>
     </row>
-    <row r="169" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B169" s="7"/>
       <c r="C169" s="7"/>
     </row>
-    <row r="170" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B170" s="7"/>
       <c r="C170" s="7"/>
     </row>
-    <row r="171" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B171" s="7"/>
       <c r="C171" s="7"/>
     </row>
-    <row r="172" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B172" s="7"/>
       <c r="C172" s="7"/>
     </row>
-    <row r="173" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B173" s="7"/>
       <c r="C173" s="7"/>
     </row>
-    <row r="174" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B174" s="7"/>
       <c r="C174" s="7"/>
     </row>
-    <row r="175" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B175" s="7"/>
       <c r="C175" s="7"/>
     </row>
-    <row r="176" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B176" s="7"/>
       <c r="C176" s="7"/>
     </row>
@@ -3679,6 +3921,22 @@
     <row r="294" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B294" s="7"/>
       <c r="C294" s="7"/>
+    </row>
+    <row r="295" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B295" s="7"/>
+      <c r="C295" s="7"/>
+    </row>
+    <row r="296" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B296" s="7"/>
+      <c r="C296" s="7"/>
+    </row>
+    <row r="297" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B297" s="7"/>
+      <c r="C297" s="7"/>
+    </row>
+    <row r="298" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B298" s="7"/>
+      <c r="C298" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
lode runner - level 11 done - 3611 ahead
</commit_message>
<xml_diff>
--- a/LodeRunner/compare.xlsx
+++ b/LodeRunner/compare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\LodeRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591030D0-5156-463C-9107-95F3AD4FF983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD57DB06-27F0-477E-B226-AD10749EBAFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="50865" yWindow="3795" windowWidth="7170" windowHeight="12990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="281">
   <si>
     <t>Place</t>
   </si>
@@ -863,6 +863,21 @@
   </si>
   <si>
     <t>10 grab ladder</t>
+  </si>
+  <si>
+    <t>10 end</t>
+  </si>
+  <si>
+    <t>11 1st move</t>
+  </si>
+  <si>
+    <t>11 end</t>
+  </si>
+  <si>
+    <t>gold = 7</t>
+  </si>
+  <si>
+    <t>12 1st move</t>
   </si>
 </sst>
 </file>
@@ -1670,11 +1685,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB48F502-AA0A-4BF9-ABA2-AA87E3F2B5E4}">
-  <dimension ref="A1:E298"/>
+  <dimension ref="A1:E299"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A45" sqref="A45"/>
+      <selection pane="bottomLeft" activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2351,54 +2366,84 @@
       <c r="E44" s="7"/>
     </row>
     <row r="45" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45" s="7"/>
-      <c r="B45" s="7"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="3" t="str">
-        <f t="shared" ref="D45:D76" si="2">IF(C45&lt;&gt;"",IF(B45&lt;&gt;"",C45-B45,"-"), "-")</f>
-        <v>-</v>
+      <c r="A45" s="45" t="s">
+        <v>276</v>
+      </c>
+      <c r="B45" s="7">
+        <v>9117</v>
+      </c>
+      <c r="C45" s="7">
+        <v>12106</v>
+      </c>
+      <c r="D45" s="3">
+        <f t="shared" ref="D45:D77" si="2">IF(C45&lt;&gt;"",IF(B45&lt;&gt;"",C45-B45,"-"), "-")</f>
+        <v>2989</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="33"/>
-      <c r="B46" s="7"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="3" t="str">
+      <c r="A46" s="45" t="s">
+        <v>277</v>
+      </c>
+      <c r="B46" s="7">
+        <v>9469</v>
+      </c>
+      <c r="C46" s="7">
+        <v>12775</v>
+      </c>
+      <c r="D46" s="3">
         <f t="shared" si="2"/>
-        <v>-</v>
+        <v>3306</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A47" s="7"/>
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="3" t="str">
+      <c r="A47" s="45" t="s">
+        <v>279</v>
+      </c>
+      <c r="B47" s="7">
+        <v>9711</v>
+      </c>
+      <c r="C47" s="7">
+        <v>13012</v>
+      </c>
+      <c r="D47" s="3">
         <f t="shared" si="2"/>
-        <v>-</v>
+        <v>3301</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A48" s="7"/>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="3" t="str">
+      <c r="A48" s="45" t="s">
+        <v>278</v>
+      </c>
+      <c r="B48" s="7">
+        <v>9777</v>
+      </c>
+      <c r="C48" s="7">
+        <v>13069</v>
+      </c>
+      <c r="D48" s="3">
         <f t="shared" si="2"/>
-        <v>-</v>
+        <v>3292</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A49" s="7"/>
-      <c r="B49" s="8"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="3" t="str">
+      <c r="A49" s="45" t="s">
+        <v>280</v>
+      </c>
+      <c r="B49" s="7">
+        <v>10127</v>
+      </c>
+      <c r="C49" s="7">
+        <v>13738</v>
+      </c>
+      <c r="D49" s="3">
         <f t="shared" si="2"/>
-        <v>-</v>
+        <v>3611</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="7"/>
-      <c r="B50" s="33"/>
-      <c r="C50" s="33"/>
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
       <c r="D50" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2406,8 +2451,8 @@
     </row>
     <row r="51" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
-      <c r="B51" s="7"/>
-      <c r="C51" s="7"/>
+      <c r="B51" s="33"/>
+      <c r="C51" s="33"/>
       <c r="D51" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2603,7 +2648,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A73" s="34"/>
+      <c r="A73" s="7"/>
       <c r="B73" s="7"/>
       <c r="C73" s="7"/>
       <c r="D73" s="3" t="str">
@@ -2630,7 +2675,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A76" s="7"/>
+      <c r="A76" s="34"/>
       <c r="B76" s="7"/>
       <c r="C76" s="7"/>
       <c r="D76" s="3" t="str">
@@ -2643,23 +2688,23 @@
       <c r="B77" s="7"/>
       <c r="C77" s="7"/>
       <c r="D77" s="3" t="str">
-        <f t="shared" ref="D77:D83" si="3">IF(C77&lt;&gt;"",IF(B77&lt;&gt;"",C77-B77,"-"), "-")</f>
+        <f t="shared" si="2"/>
         <v>-</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="7"/>
-      <c r="B78" s="9"/>
-      <c r="C78" s="9"/>
+      <c r="B78" s="7"/>
+      <c r="C78" s="7"/>
       <c r="D78" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="D78:D84" si="3">IF(C78&lt;&gt;"",IF(B78&lt;&gt;"",C78-B78,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="7"/>
-      <c r="B79" s="7"/>
-      <c r="C79" s="7"/>
+      <c r="B79" s="9"/>
+      <c r="C79" s="9"/>
       <c r="D79" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
@@ -2667,8 +2712,8 @@
     </row>
     <row r="80" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="7"/>
-      <c r="B80" s="9"/>
-      <c r="C80" s="9"/>
+      <c r="B80" s="7"/>
+      <c r="C80" s="7"/>
       <c r="D80" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
@@ -2676,8 +2721,8 @@
     </row>
     <row r="81" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="7"/>
-      <c r="B81" s="7"/>
-      <c r="C81" s="7"/>
+      <c r="B81" s="9"/>
+      <c r="C81" s="9"/>
       <c r="D81" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
@@ -2693,7 +2738,7 @@
       </c>
     </row>
     <row r="83" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A83" s="5"/>
+      <c r="A83" s="7"/>
       <c r="B83" s="7"/>
       <c r="C83" s="7"/>
       <c r="D83" s="3" t="str">
@@ -2706,7 +2751,7 @@
       <c r="B84" s="7"/>
       <c r="C84" s="7"/>
       <c r="D84" s="3" t="str">
-        <f t="shared" ref="D84:D152" si="4">IF(C84&lt;&gt;"",IF(B84&lt;&gt;"",C84-B84,"-"), "-")</f>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
     </row>
@@ -2715,7 +2760,7 @@
       <c r="B85" s="7"/>
       <c r="C85" s="7"/>
       <c r="D85" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="D85:D153" si="4">IF(C85&lt;&gt;"",IF(B85&lt;&gt;"",C85-B85,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
@@ -2756,7 +2801,7 @@
       </c>
     </row>
     <row r="90" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A90" s="7"/>
+      <c r="A90" s="5"/>
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
       <c r="D90" s="3" t="str">
@@ -2774,7 +2819,7 @@
       </c>
     </row>
     <row r="92" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A92" s="34"/>
+      <c r="A92" s="7"/>
       <c r="B92" s="7"/>
       <c r="C92" s="7"/>
       <c r="D92" s="3" t="str">
@@ -2783,7 +2828,7 @@
       </c>
     </row>
     <row r="93" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A93" s="7"/>
+      <c r="A93" s="34"/>
       <c r="B93" s="7"/>
       <c r="C93" s="7"/>
       <c r="D93" s="3" t="str">
@@ -2792,7 +2837,7 @@
       </c>
     </row>
     <row r="94" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A94" s="5"/>
+      <c r="A94" s="7"/>
       <c r="B94" s="7"/>
       <c r="C94" s="7"/>
       <c r="D94" s="3" t="str">
@@ -2946,8 +2991,8 @@
     </row>
     <row r="111" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A111" s="5"/>
-      <c r="B111" s="10"/>
-      <c r="C111" s="10"/>
+      <c r="B111" s="7"/>
+      <c r="C111" s="7"/>
       <c r="D111" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
@@ -2955,15 +3000,15 @@
     </row>
     <row r="112" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A112" s="5"/>
-      <c r="B112" s="7"/>
-      <c r="C112" s="7"/>
+      <c r="B112" s="10"/>
+      <c r="C112" s="10"/>
       <c r="D112" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A113" s="35"/>
+      <c r="A113" s="5"/>
       <c r="B113" s="7"/>
       <c r="C113" s="7"/>
       <c r="D113" s="3" t="str">
@@ -2972,7 +3017,7 @@
       </c>
     </row>
     <row r="114" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A114" s="5"/>
+      <c r="A114" s="35"/>
       <c r="B114" s="7"/>
       <c r="C114" s="7"/>
       <c r="D114" s="3" t="str">
@@ -3011,7 +3056,10 @@
       <c r="A118" s="5"/>
       <c r="B118" s="7"/>
       <c r="C118" s="7"/>
-      <c r="D118" s="3"/>
+      <c r="D118" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="119" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A119" s="5"/>
@@ -3026,22 +3074,19 @@
       <c r="D120" s="3"/>
     </row>
     <row r="121" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A121" s="5" t="s">
+      <c r="A121" s="5"/>
+      <c r="B121" s="7"/>
+      <c r="C121" s="7"/>
+      <c r="D121" s="3"/>
+    </row>
+    <row r="122" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A122" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B121" s="7"/>
-      <c r="C121" s="7">
+      <c r="B122" s="7"/>
+      <c r="C122" s="7">
         <v>63782</v>
       </c>
-      <c r="D121" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A122" s="7"/>
-      <c r="B122" s="7"/>
-      <c r="C122" s="7"/>
       <c r="D122" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
@@ -3322,7 +3367,7 @@
       <c r="B153" s="7"/>
       <c r="C153" s="7"/>
       <c r="D153" s="3" t="str">
-        <f t="shared" ref="D153:D157" si="5">IF(C153&lt;&gt;"",IF(B153&lt;&gt;"",C153-B153,"-"), "-")</f>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
     </row>
@@ -3331,7 +3376,7 @@
       <c r="B154" s="7"/>
       <c r="C154" s="7"/>
       <c r="D154" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="D154:D158" si="5">IF(C154&lt;&gt;"",IF(B154&lt;&gt;"",C154-B154,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
@@ -3367,7 +3412,7 @@
       <c r="B158" s="7"/>
       <c r="C158" s="7"/>
       <c r="D158" s="3" t="str">
-        <f t="shared" ref="D158:D159" si="6">IF(C158&lt;&gt;"",IF(B158&lt;&gt;"",B158-C158,"-"), "-")</f>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
     </row>
@@ -3376,7 +3421,7 @@
       <c r="B159" s="7"/>
       <c r="C159" s="7"/>
       <c r="D159" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="D159:D160" si="6">IF(C159&lt;&gt;"",IF(B159&lt;&gt;"",B159-C159,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
@@ -3384,6 +3429,10 @@
       <c r="A160" s="7"/>
       <c r="B160" s="7"/>
       <c r="C160" s="7"/>
+      <c r="D160" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="161" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A161" s="7"/>
@@ -3391,6 +3440,7 @@
       <c r="C161" s="7"/>
     </row>
     <row r="162" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A162" s="7"/>
       <c r="B162" s="7"/>
       <c r="C162" s="7"/>
     </row>
@@ -3937,6 +3987,10 @@
     <row r="298" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B298" s="7"/>
       <c r="C298" s="7"/>
+    </row>
+    <row r="299" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B299" s="7"/>
+      <c r="C299" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>